<commit_message>
More FR data; fix allende_scraper_france_streets
</commit_message>
<xml_diff>
--- a/a-place-for-salvador-allende/countries/France_all.xlsx
+++ b/a-place-for-salvador-allende/countries/France_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GoGro\Desktop\Repos\datasets-of-interest\a-place-for-salvador-allende\countries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1342C2-01B8-42EC-8908-0154793EEF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700CBC49-7B01-45DA-9548-8C7BD86F7B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33480" yWindow="2925" windowWidth="29040" windowHeight="17790" xr2:uid="{FB19995C-71E8-4436-B5BB-733167ED68ED}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="534">
   <si>
     <t>id</t>
   </si>
@@ -947,6 +947,751 @@
   </si>
   <si>
     <t>https://goo.gl/maps/W7Qn5h1aB6sKN3bx6</t>
+  </si>
+  <si>
+    <t>Moselle</t>
+  </si>
+  <si>
+    <t>Thionville</t>
+  </si>
+  <si>
+    <t>Audun-le-Tiche</t>
+  </si>
+  <si>
+    <t>57390</t>
+  </si>
+  <si>
+    <t>Avenue Salvador ALLENDE
+1908_1973
+Président du gouvernement d'Unité Populaire du Chili 
+Assassiné lors du coup d'État fasciste du 11 septembre 1973</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/201512050</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/dGBMiyhsfGsQ2rtP6</t>
+  </si>
+  <si>
+    <t>Nièvre</t>
+  </si>
+  <si>
+    <t>Nevers</t>
+  </si>
+  <si>
+    <t>Varennes-Vauzelles</t>
+  </si>
+  <si>
+    <t>58640</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/652447660</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/JyS9w1GSiorUS4EaA</t>
+  </si>
+  <si>
+    <t>Ronchin</t>
+  </si>
+  <si>
+    <t>59790</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/42585610</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/d6qD3JFdPAypS2Sa9</t>
+  </si>
+  <si>
+    <t>Haute-Vienne</t>
+  </si>
+  <si>
+    <t>Limoges</t>
+  </si>
+  <si>
+    <t>Le Palais-sur-Vienne</t>
+  </si>
+  <si>
+    <t>87410</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/58682412</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/zKvvXXixVcG4huBN9</t>
+  </si>
+  <si>
+    <t>Pas-de-Calais</t>
+  </si>
+  <si>
+    <t>Lens</t>
+  </si>
+  <si>
+    <t>62300</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/82532074</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/yjovmxFZWoHo3ZHK7</t>
+  </si>
+  <si>
+    <t>Puy-de-Dôme</t>
+  </si>
+  <si>
+    <t>Riom</t>
+  </si>
+  <si>
+    <t>63200</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/72112462</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/yLg1VbBVSdM11tT39</t>
+  </si>
+  <si>
+    <t>Clermont-Ferrand</t>
+  </si>
+  <si>
+    <t>Cournon-d'Auvergne</t>
+  </si>
+  <si>
+    <t>63800</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/504240208</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/HHjVXDKaqgDQ874T9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2012/09/11/588-cournon-d-auvergne-francia</t>
+  </si>
+  <si>
+    <t>Rhône</t>
+  </si>
+  <si>
+    <t>Métropole de Lyon</t>
+  </si>
+  <si>
+    <t>Décines-Charpieu</t>
+  </si>
+  <si>
+    <t>69150</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/22690262</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/qaHGAAjqPHBpeSCf9</t>
+  </si>
+  <si>
+    <t>Saint-Priest</t>
+  </si>
+  <si>
+    <t>69800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St Priest 
+Avenue Salvador ALLENDE 
+Homme d'État chilien 1908-1973 </t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/1851761337</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/3s7V14w7q1yxbrHD7</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/02/13/146-saint-priest-francia</t>
+  </si>
+  <si>
+    <t>Saône-et-Loire</t>
+  </si>
+  <si>
+    <t>Chalon-sur-Saône</t>
+  </si>
+  <si>
+    <t>Plateau Saint-Jean</t>
+  </si>
+  <si>
+    <t>71100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avenue Salvador ALLENDE 
+Homme d'État Chilien 
+1908 - 1973 </t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/3043044207</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/kAqpHvU475WhZ4HM8</t>
+  </si>
+  <si>
+    <t>Torcy</t>
+  </si>
+  <si>
+    <t>Pôle commercial Bay 1</t>
+  </si>
+  <si>
+    <t>77200</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/27619579</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/SDxmR5gHRsPJSqSQ8</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/09/24/399-torcy-francia</t>
+  </si>
+  <si>
+    <t>Yvelines</t>
+  </si>
+  <si>
+    <t>Versailles</t>
+  </si>
+  <si>
+    <t>Trappes</t>
+  </si>
+  <si>
+    <t>78190</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/26616077</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/vGvVeLfomrX6wzVL9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/07/29/242-trappes-francia</t>
+  </si>
+  <si>
+    <t>Deux-Sèvres</t>
+  </si>
+  <si>
+    <t>Niort</t>
+  </si>
+  <si>
+    <t>Tour Chabot Gavacherie</t>
+  </si>
+  <si>
+    <t>79000</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/369283703</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/oCCXqTSYXTnJLetW7</t>
+  </si>
+  <si>
+    <t>Somme</t>
+  </si>
+  <si>
+    <t>Amiens</t>
+  </si>
+  <si>
+    <t>80044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rue Salvador Allende 
+Président de la République du Chili 
+1970-1973 </t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/26675184</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/WzHF5jdb2SWKbSaX7</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/07/16/231-amiens-francia</t>
+  </si>
+  <si>
+    <t>Rivery</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/36970001</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/7o5D2c2aBKoEV9u78</t>
+  </si>
+  <si>
+    <t>Rue du Président Allende</t>
+  </si>
+  <si>
+    <t>Corbie</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/32517854</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/WmeqQLCHoxcgvSV99</t>
+  </si>
+  <si>
+    <t>Var</t>
+  </si>
+  <si>
+    <t>Draguignan</t>
+  </si>
+  <si>
+    <t>83300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avenue Salvador Allende 
+Ancien Président de la République du Chili </t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/156414888</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/tZ6NRWEmr57mD8LFA</t>
+  </si>
+  <si>
+    <t>Toulon</t>
+  </si>
+  <si>
+    <t>La Seyne-sur-Mer</t>
+  </si>
+  <si>
+    <t>83500</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/1015280723</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/sLk2efxLqVfViu17A</t>
+  </si>
+  <si>
+    <t>Carpentras</t>
+  </si>
+  <si>
+    <t>Bollène</t>
+  </si>
+  <si>
+    <t>84500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avenue Salvador ALLENDE 
+Président de la République du Chili 
+de 1970 à 1973 </t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/8752531601</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/ncuKtivUfB6NYkt19</t>
+  </si>
+  <si>
+    <t>Eymoutiers</t>
+  </si>
+  <si>
+    <t>87120</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/296084414</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/pyHJewZp38H59aMx7</t>
+  </si>
+  <si>
+    <t>Vosges</t>
+  </si>
+  <si>
+    <t>Épinal</t>
+  </si>
+  <si>
+    <t>Saut le Cerf</t>
+  </si>
+  <si>
+    <t>88000</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/99551729</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/bjiRdBWzF9qLjxWv8</t>
+  </si>
+  <si>
+    <t>Palaiseau</t>
+  </si>
+  <si>
+    <t>Saulx-les-Chartreux</t>
+  </si>
+  <si>
+    <t>91160</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/1022672088</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/fAtVGCQdPZuP8iGk9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/07/06/220-saulx-les-chartreux-francia</t>
+  </si>
+  <si>
+    <t>Le Raincy</t>
+  </si>
+  <si>
+    <t>Sevran</t>
+  </si>
+  <si>
+    <t>93270</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/32539285</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/SSZBh5y6fTC9rB4n7</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/09/05/259-sevran-francia</t>
+  </si>
+  <si>
+    <t>Épinay-sur-Seine</t>
+  </si>
+  <si>
+    <t>93800</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/70192355</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/yVjQ3rACmHKyFq898</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/04/11/177-epinay-sur-seine-francia</t>
+  </si>
+  <si>
+    <t>Nogent-sur-Marne</t>
+  </si>
+  <si>
+    <t>Champigny-sur-Marne</t>
+  </si>
+  <si>
+    <t>94500</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/110069648</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/J8X3tUQ3JCyokq4E8</t>
+  </si>
+  <si>
+    <t>Val-d'Oise</t>
+  </si>
+  <si>
+    <t>Argenteuil</t>
+  </si>
+  <si>
+    <t>Taverny</t>
+  </si>
+  <si>
+    <t>95150</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/39520420</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/WbCQMTdQciagMaZ16</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/07/01/213-taverny-francia</t>
+  </si>
+  <si>
+    <t>Avenue Salvador Allende Gossens</t>
+  </si>
+  <si>
+    <t>Reims</t>
+  </si>
+  <si>
+    <t>51100</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/32117167</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/qXi9PxbM1d8eZfJDA</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2011/02/23/514-reims-francia</t>
+  </si>
+  <si>
+    <t>14th Arrondissement</t>
+  </si>
+  <si>
+    <t>13014</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/707440336</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/qdhJ82zsAx3wTBqn7</t>
+  </si>
+  <si>
+    <t>La Ciotat</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/432140134</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/TJDPJYzWA1HgfGscA</t>
+  </si>
+  <si>
+    <t>Place Salvador Allende</t>
+  </si>
+  <si>
+    <t>park</t>
+  </si>
+  <si>
+    <t>Septèmes-les-Vallons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Place Salvador Allende 
+1908 - 1973 
+Président de la République du Chili 
+Mort les armes à la main pour la défense de la democratie </t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/548307641</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/rZKPjH8UZwWNWFfN6</t>
+  </si>
+  <si>
+    <t>Boulevard du Président Salvador Allende</t>
+  </si>
+  <si>
+    <t>03100</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/73565861</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/N7gqJJ1yvHiTaAAH9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2012/08/19/577-montlucon-francia</t>
+  </si>
+  <si>
+    <t>Boulevard du Président Allende</t>
+  </si>
+  <si>
+    <t>Domérat</t>
+  </si>
+  <si>
+    <t>03410</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/877949175</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/UNkYQDPQ1KGa78td9</t>
+  </si>
+  <si>
+    <t>Saint-Mitre-les-Remparts</t>
+  </si>
+  <si>
+    <t>13920</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/555156595</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/NnMLMuhxmvcuU9ms7</t>
+  </si>
+  <si>
+    <t>Eure</t>
+  </si>
+  <si>
+    <t>Évreux</t>
+  </si>
+  <si>
+    <t>Le Clos au Duc</t>
+  </si>
+  <si>
+    <t>27000</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/845077262</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/XxDuUuzs5mfibTbK6</t>
+  </si>
+  <si>
+    <t>Boulevard Président Allende</t>
+  </si>
+  <si>
+    <t>Quimper</t>
+  </si>
+  <si>
+    <t>Moulin de Kermahonnet</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/905032942</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/ZuXFr9Qdc5ukcMCX8</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2012/07/09/566-quimper-francia</t>
+  </si>
+  <si>
+    <t>Arras</t>
+  </si>
+  <si>
+    <t>62000</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/316774229</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/XGjwSff9ZekaSPEAA</t>
+  </si>
+  <si>
+    <t>Boulevard Salvador Allende</t>
+  </si>
+  <si>
+    <t>Aix-en-Provence</t>
+  </si>
+  <si>
+    <t>Gréasque</t>
+  </si>
+  <si>
+    <t>13850</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/90745450</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/t3hab5QmwK7KAuWQA</t>
+  </si>
+  <si>
+    <t>Calvados</t>
+  </si>
+  <si>
+    <t>Caen</t>
+  </si>
+  <si>
+    <t>Blainville-sur-Orne</t>
+  </si>
+  <si>
+    <t>14550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rue Salvador Allende 
+Président du Chili 1908-1973 </t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/83603741</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/8L9Yjp2qDpCAxSC16</t>
+  </si>
+  <si>
+    <t>Charente</t>
+  </si>
+  <si>
+    <t>Angoulême</t>
+  </si>
+  <si>
+    <t>16000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boulevard Salvador ALLENDE 
+(1908-1973) 
+Président de la République du Chili 
+de 1970 à 1973 </t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/128634354</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/YBRTXRZEfHRDgSW46</t>
+  </si>
+  <si>
+    <t>Boluevard/Place Salvador Allende</t>
+  </si>
+  <si>
+    <t>Vierzon</t>
+  </si>
+  <si>
+    <t>Le Desert</t>
+  </si>
+  <si>
+    <t>18100</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/40099765</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/LaJCjuHsf8scyPnL7</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2012/09/07/586-vierzon-francia</t>
+  </si>
+  <si>
+    <t>Chevigny-Saint-Sauveur</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/646869464</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/ak4pyjiLG8FBMveu5</t>
+  </si>
+  <si>
+    <t>Doubs</t>
+  </si>
+  <si>
+    <t>Besançon</t>
+  </si>
+  <si>
+    <t>Cassin</t>
+  </si>
+  <si>
+    <t>25000</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/1146186361</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/NBu4jWkj21m5mAL67</t>
+  </si>
+  <si>
+    <t>Douarnenez</t>
+  </si>
+  <si>
+    <t>29100</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/40001773</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/g4vrfmHNp66qP54M8</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2012/08/22/580-douarnenez-francia</t>
+  </si>
+  <si>
+    <t>Langon</t>
+  </si>
+  <si>
+    <t>La Carrelasse</t>
+  </si>
+  <si>
+    <t>33210</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/31252655</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/y2pmTNVS1qpVAn2F9</t>
+  </si>
+  <si>
+    <t>Rue du Pont Neuf</t>
   </si>
 </sst>
 </file>
@@ -1014,12 +1759,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1346,10 +2094,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F527D2B3-F30A-4BB6-B445-B84E88C49493}">
-  <dimension ref="A1:Y41"/>
+  <dimension ref="A1:Y85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3947,6 +4696,2719 @@
         <v>291</v>
       </c>
       <c r="Y41" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42" t="s">
+        <v>61</v>
+      </c>
+      <c r="H42" t="s">
+        <v>292</v>
+      </c>
+      <c r="I42" t="s">
+        <v>293</v>
+      </c>
+      <c r="J42" t="s">
+        <v>294</v>
+      </c>
+      <c r="K42" t="s">
+        <v>295</v>
+      </c>
+      <c r="L42">
+        <v>49.475085900000003</v>
+      </c>
+      <c r="M42">
+        <v>5.9497343999999996</v>
+      </c>
+      <c r="N42">
+        <v>2009</v>
+      </c>
+      <c r="O42">
+        <v>5</v>
+      </c>
+      <c r="P42">
+        <v>13</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>35</v>
+      </c>
+      <c r="R42" t="s">
+        <v>296</v>
+      </c>
+      <c r="S42" t="s">
+        <v>37</v>
+      </c>
+      <c r="V42">
+        <v>1</v>
+      </c>
+      <c r="W42" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="X42" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y42" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" t="s">
+        <v>28</v>
+      </c>
+      <c r="F43" t="s">
+        <v>29</v>
+      </c>
+      <c r="G43" t="s">
+        <v>234</v>
+      </c>
+      <c r="H43" t="s">
+        <v>299</v>
+      </c>
+      <c r="I43" t="s">
+        <v>300</v>
+      </c>
+      <c r="J43" t="s">
+        <v>301</v>
+      </c>
+      <c r="K43" t="s">
+        <v>302</v>
+      </c>
+      <c r="L43">
+        <v>47.0100306</v>
+      </c>
+      <c r="M43">
+        <v>3.1383329999999998</v>
+      </c>
+      <c r="N43">
+        <v>2009</v>
+      </c>
+      <c r="O43">
+        <v>5</v>
+      </c>
+      <c r="P43">
+        <v>13</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>35</v>
+      </c>
+      <c r="V43">
+        <v>1</v>
+      </c>
+      <c r="W43" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="X43" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="Y43" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" t="s">
+        <v>28</v>
+      </c>
+      <c r="F44" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" t="s">
+        <v>123</v>
+      </c>
+      <c r="H44" t="s">
+        <v>124</v>
+      </c>
+      <c r="I44" t="s">
+        <v>125</v>
+      </c>
+      <c r="J44" t="s">
+        <v>305</v>
+      </c>
+      <c r="K44" t="s">
+        <v>306</v>
+      </c>
+      <c r="L44">
+        <v>50.598182399999999</v>
+      </c>
+      <c r="M44">
+        <v>3.0891251999999998</v>
+      </c>
+      <c r="N44">
+        <v>2008</v>
+      </c>
+      <c r="O44">
+        <v>5</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>47</v>
+      </c>
+      <c r="V44">
+        <v>1</v>
+      </c>
+      <c r="W44" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="X44" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="Y44" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" t="s">
+        <v>29</v>
+      </c>
+      <c r="G45" t="s">
+        <v>42</v>
+      </c>
+      <c r="H45" t="s">
+        <v>309</v>
+      </c>
+      <c r="I45" t="s">
+        <v>310</v>
+      </c>
+      <c r="J45" t="s">
+        <v>311</v>
+      </c>
+      <c r="K45" t="s">
+        <v>312</v>
+      </c>
+      <c r="L45">
+        <v>45.869230000000002</v>
+      </c>
+      <c r="M45">
+        <v>1.3098399999999999</v>
+      </c>
+      <c r="N45">
+        <v>2009</v>
+      </c>
+      <c r="O45">
+        <v>5</v>
+      </c>
+      <c r="P45">
+        <v>13</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>35</v>
+      </c>
+      <c r="V45">
+        <v>1</v>
+      </c>
+      <c r="W45" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="X45" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="Y45" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" t="s">
+        <v>28</v>
+      </c>
+      <c r="F46" t="s">
+        <v>29</v>
+      </c>
+      <c r="G46" t="s">
+        <v>123</v>
+      </c>
+      <c r="H46" t="s">
+        <v>315</v>
+      </c>
+      <c r="I46" t="s">
+        <v>316</v>
+      </c>
+      <c r="K46" t="s">
+        <v>317</v>
+      </c>
+      <c r="L46">
+        <v>50.440590999999998</v>
+      </c>
+      <c r="M46">
+        <v>2.8310951000000002</v>
+      </c>
+      <c r="N46">
+        <v>2008</v>
+      </c>
+      <c r="O46">
+        <v>7</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>47</v>
+      </c>
+      <c r="V46">
+        <v>1</v>
+      </c>
+      <c r="W46" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="X46" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="Y46" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" t="s">
+        <v>28</v>
+      </c>
+      <c r="F47" t="s">
+        <v>29</v>
+      </c>
+      <c r="G47" t="s">
+        <v>86</v>
+      </c>
+      <c r="H47" t="s">
+        <v>320</v>
+      </c>
+      <c r="I47" t="s">
+        <v>321</v>
+      </c>
+      <c r="K47" t="s">
+        <v>322</v>
+      </c>
+      <c r="L47">
+        <v>45.889099999999999</v>
+      </c>
+      <c r="M47">
+        <v>3.1353599999999999</v>
+      </c>
+      <c r="N47">
+        <v>2008</v>
+      </c>
+      <c r="O47">
+        <v>7</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>47</v>
+      </c>
+      <c r="V47">
+        <v>1</v>
+      </c>
+      <c r="W47" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="X47" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="Y47" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" t="s">
+        <v>28</v>
+      </c>
+      <c r="F48" t="s">
+        <v>29</v>
+      </c>
+      <c r="G48" t="s">
+        <v>86</v>
+      </c>
+      <c r="H48" t="s">
+        <v>320</v>
+      </c>
+      <c r="I48" t="s">
+        <v>325</v>
+      </c>
+      <c r="J48" t="s">
+        <v>326</v>
+      </c>
+      <c r="K48" t="s">
+        <v>327</v>
+      </c>
+      <c r="L48">
+        <v>45.741655100000003</v>
+      </c>
+      <c r="M48">
+        <v>3.2085544000000001</v>
+      </c>
+      <c r="N48">
+        <v>2009</v>
+      </c>
+      <c r="O48">
+        <v>5</v>
+      </c>
+      <c r="P48">
+        <v>13</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>35</v>
+      </c>
+      <c r="V48">
+        <v>1</v>
+      </c>
+      <c r="W48" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="X48" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="Y48" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="49" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" t="s">
+        <v>28</v>
+      </c>
+      <c r="F49" t="s">
+        <v>29</v>
+      </c>
+      <c r="G49" t="s">
+        <v>86</v>
+      </c>
+      <c r="H49" t="s">
+        <v>331</v>
+      </c>
+      <c r="I49" t="s">
+        <v>332</v>
+      </c>
+      <c r="J49" t="s">
+        <v>333</v>
+      </c>
+      <c r="K49" t="s">
+        <v>334</v>
+      </c>
+      <c r="L49">
+        <v>45.766984999999998</v>
+      </c>
+      <c r="M49">
+        <v>4.9711097999999998</v>
+      </c>
+      <c r="N49">
+        <v>2008</v>
+      </c>
+      <c r="O49">
+        <v>6</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>47</v>
+      </c>
+      <c r="V49">
+        <v>1</v>
+      </c>
+      <c r="W49" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="X49" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="Y49" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>114</v>
+      </c>
+      <c r="C50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" t="s">
+        <v>28</v>
+      </c>
+      <c r="F50" t="s">
+        <v>29</v>
+      </c>
+      <c r="G50" t="s">
+        <v>86</v>
+      </c>
+      <c r="H50" t="s">
+        <v>331</v>
+      </c>
+      <c r="I50" t="s">
+        <v>332</v>
+      </c>
+      <c r="J50" t="s">
+        <v>337</v>
+      </c>
+      <c r="K50" t="s">
+        <v>338</v>
+      </c>
+      <c r="L50">
+        <v>45.703432599999999</v>
+      </c>
+      <c r="M50">
+        <v>4.9349246000000004</v>
+      </c>
+      <c r="N50">
+        <v>2008</v>
+      </c>
+      <c r="O50">
+        <v>2</v>
+      </c>
+      <c r="P50">
+        <v>13</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>35</v>
+      </c>
+      <c r="R50" t="s">
+        <v>339</v>
+      </c>
+      <c r="S50" t="s">
+        <v>37</v>
+      </c>
+      <c r="V50">
+        <v>1</v>
+      </c>
+      <c r="W50" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="X50" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="Y50" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="51" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" t="s">
+        <v>28</v>
+      </c>
+      <c r="F51" t="s">
+        <v>29</v>
+      </c>
+      <c r="G51" t="s">
+        <v>234</v>
+      </c>
+      <c r="H51" t="s">
+        <v>343</v>
+      </c>
+      <c r="I51" t="s">
+        <v>344</v>
+      </c>
+      <c r="J51" t="s">
+        <v>345</v>
+      </c>
+      <c r="K51" t="s">
+        <v>346</v>
+      </c>
+      <c r="L51">
+        <v>46.805750000000003</v>
+      </c>
+      <c r="M51">
+        <v>4.8538699999999997</v>
+      </c>
+      <c r="N51">
+        <v>2009</v>
+      </c>
+      <c r="O51">
+        <v>5</v>
+      </c>
+      <c r="P51">
+        <v>13</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>35</v>
+      </c>
+      <c r="R51" t="s">
+        <v>347</v>
+      </c>
+      <c r="S51" t="s">
+        <v>37</v>
+      </c>
+      <c r="V51">
+        <v>1</v>
+      </c>
+      <c r="W51" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="X51" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Y51" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" t="s">
+        <v>28</v>
+      </c>
+      <c r="F52" t="s">
+        <v>29</v>
+      </c>
+      <c r="G52" t="s">
+        <v>30</v>
+      </c>
+      <c r="H52" t="s">
+        <v>180</v>
+      </c>
+      <c r="I52" t="s">
+        <v>350</v>
+      </c>
+      <c r="J52" t="s">
+        <v>351</v>
+      </c>
+      <c r="K52" t="s">
+        <v>352</v>
+      </c>
+      <c r="L52">
+        <v>48.84366</v>
+      </c>
+      <c r="M52">
+        <v>2.6546799999999999</v>
+      </c>
+      <c r="N52">
+        <v>2008</v>
+      </c>
+      <c r="O52">
+        <v>7</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>47</v>
+      </c>
+      <c r="V52">
+        <v>1</v>
+      </c>
+      <c r="W52" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="X52" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="Y52" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="53" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" t="s">
+        <v>28</v>
+      </c>
+      <c r="F53" t="s">
+        <v>29</v>
+      </c>
+      <c r="G53" t="s">
+        <v>30</v>
+      </c>
+      <c r="H53" t="s">
+        <v>356</v>
+      </c>
+      <c r="I53" t="s">
+        <v>357</v>
+      </c>
+      <c r="J53" t="s">
+        <v>358</v>
+      </c>
+      <c r="K53" t="s">
+        <v>359</v>
+      </c>
+      <c r="L53">
+        <v>48.786344900000003</v>
+      </c>
+      <c r="M53">
+        <v>1.9801274</v>
+      </c>
+      <c r="N53">
+        <v>2008</v>
+      </c>
+      <c r="O53">
+        <v>7</v>
+      </c>
+      <c r="P53">
+        <v>29</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>35</v>
+      </c>
+      <c r="V53">
+        <v>1</v>
+      </c>
+      <c r="W53" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="X53" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="Y53" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="54" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" t="s">
+        <v>28</v>
+      </c>
+      <c r="F54" t="s">
+        <v>29</v>
+      </c>
+      <c r="G54" t="s">
+        <v>42</v>
+      </c>
+      <c r="H54" t="s">
+        <v>363</v>
+      </c>
+      <c r="I54" t="s">
+        <v>364</v>
+      </c>
+      <c r="J54" t="s">
+        <v>365</v>
+      </c>
+      <c r="K54" t="s">
+        <v>366</v>
+      </c>
+      <c r="L54">
+        <v>46.326639999999998</v>
+      </c>
+      <c r="M54">
+        <v>-0.48635</v>
+      </c>
+      <c r="N54">
+        <v>2009</v>
+      </c>
+      <c r="O54">
+        <v>5</v>
+      </c>
+      <c r="P54">
+        <v>13</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>35</v>
+      </c>
+      <c r="V54">
+        <v>1</v>
+      </c>
+      <c r="W54" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="X54" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y54" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" t="s">
+        <v>29</v>
+      </c>
+      <c r="G55" t="s">
+        <v>123</v>
+      </c>
+      <c r="H55" t="s">
+        <v>369</v>
+      </c>
+      <c r="I55" t="s">
+        <v>370</v>
+      </c>
+      <c r="K55" t="s">
+        <v>371</v>
+      </c>
+      <c r="L55">
+        <v>49.896963800000002</v>
+      </c>
+      <c r="M55">
+        <v>2.2827438</v>
+      </c>
+      <c r="N55">
+        <v>2008</v>
+      </c>
+      <c r="O55">
+        <v>7</v>
+      </c>
+      <c r="P55">
+        <v>16</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>35</v>
+      </c>
+      <c r="R55" t="s">
+        <v>372</v>
+      </c>
+      <c r="S55" t="s">
+        <v>37</v>
+      </c>
+      <c r="V55">
+        <v>1</v>
+      </c>
+      <c r="W55" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="X55" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="Y55" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="56" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" t="s">
+        <v>29</v>
+      </c>
+      <c r="G56" t="s">
+        <v>123</v>
+      </c>
+      <c r="H56" t="s">
+        <v>369</v>
+      </c>
+      <c r="I56" t="s">
+        <v>370</v>
+      </c>
+      <c r="J56" t="s">
+        <v>376</v>
+      </c>
+      <c r="K56" s="3">
+        <v>80136</v>
+      </c>
+      <c r="L56">
+        <v>49.906790000000001</v>
+      </c>
+      <c r="M56">
+        <v>2.3318699999999999</v>
+      </c>
+      <c r="N56">
+        <v>2009</v>
+      </c>
+      <c r="O56">
+        <v>5</v>
+      </c>
+      <c r="P56">
+        <v>13</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>35</v>
+      </c>
+      <c r="V56">
+        <v>1</v>
+      </c>
+      <c r="W56" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="X56" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="Y56" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>379</v>
+      </c>
+      <c r="C57" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" t="s">
+        <v>28</v>
+      </c>
+      <c r="F57" t="s">
+        <v>29</v>
+      </c>
+      <c r="G57" t="s">
+        <v>123</v>
+      </c>
+      <c r="H57" t="s">
+        <v>369</v>
+      </c>
+      <c r="I57" t="s">
+        <v>370</v>
+      </c>
+      <c r="J57" t="s">
+        <v>380</v>
+      </c>
+      <c r="K57" s="3">
+        <v>80800</v>
+      </c>
+      <c r="L57">
+        <v>49.918019999999999</v>
+      </c>
+      <c r="M57">
+        <v>2.5190399999999999</v>
+      </c>
+      <c r="N57">
+        <v>2008</v>
+      </c>
+      <c r="O57">
+        <v>8</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>47</v>
+      </c>
+      <c r="V57">
+        <v>1</v>
+      </c>
+      <c r="W57" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="X57" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="Y57" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" t="s">
+        <v>28</v>
+      </c>
+      <c r="F58" t="s">
+        <v>29</v>
+      </c>
+      <c r="G58" t="s">
+        <v>77</v>
+      </c>
+      <c r="H58" t="s">
+        <v>383</v>
+      </c>
+      <c r="I58" t="s">
+        <v>384</v>
+      </c>
+      <c r="K58" t="s">
+        <v>385</v>
+      </c>
+      <c r="L58">
+        <v>43.526830699999998</v>
+      </c>
+      <c r="M58">
+        <v>6.4367517000000003</v>
+      </c>
+      <c r="N58">
+        <v>2009</v>
+      </c>
+      <c r="O58">
+        <v>5</v>
+      </c>
+      <c r="P58">
+        <v>13</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>35</v>
+      </c>
+      <c r="R58" t="s">
+        <v>386</v>
+      </c>
+      <c r="S58" t="s">
+        <v>37</v>
+      </c>
+      <c r="V58">
+        <v>1</v>
+      </c>
+      <c r="W58" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="X58" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="Y58" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" t="s">
+        <v>28</v>
+      </c>
+      <c r="F59" t="s">
+        <v>29</v>
+      </c>
+      <c r="G59" t="s">
+        <v>77</v>
+      </c>
+      <c r="H59" t="s">
+        <v>383</v>
+      </c>
+      <c r="I59" t="s">
+        <v>389</v>
+      </c>
+      <c r="J59" t="s">
+        <v>390</v>
+      </c>
+      <c r="K59" t="s">
+        <v>391</v>
+      </c>
+      <c r="L59">
+        <v>43.0892342</v>
+      </c>
+      <c r="M59">
+        <v>5.8814754999999996</v>
+      </c>
+      <c r="N59">
+        <v>2008</v>
+      </c>
+      <c r="O59">
+        <v>9</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>47</v>
+      </c>
+      <c r="V59">
+        <v>1</v>
+      </c>
+      <c r="W59" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="X59" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="Y59" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" t="s">
+        <v>28</v>
+      </c>
+      <c r="F60" t="s">
+        <v>29</v>
+      </c>
+      <c r="G60" t="s">
+        <v>77</v>
+      </c>
+      <c r="H60" t="s">
+        <v>78</v>
+      </c>
+      <c r="I60" t="s">
+        <v>394</v>
+      </c>
+      <c r="J60" t="s">
+        <v>395</v>
+      </c>
+      <c r="K60" t="s">
+        <v>396</v>
+      </c>
+      <c r="L60">
+        <v>44.288409999999999</v>
+      </c>
+      <c r="M60">
+        <v>4.75237</v>
+      </c>
+      <c r="N60">
+        <v>2009</v>
+      </c>
+      <c r="O60">
+        <v>1</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>47</v>
+      </c>
+      <c r="R60" t="s">
+        <v>397</v>
+      </c>
+      <c r="S60" t="s">
+        <v>37</v>
+      </c>
+      <c r="V60">
+        <v>1</v>
+      </c>
+      <c r="W60" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="X60" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="Y60" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>114</v>
+      </c>
+      <c r="C61" t="s">
+        <v>26</v>
+      </c>
+      <c r="D61" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" t="s">
+        <v>28</v>
+      </c>
+      <c r="F61" t="s">
+        <v>29</v>
+      </c>
+      <c r="G61" t="s">
+        <v>42</v>
+      </c>
+      <c r="H61" t="s">
+        <v>309</v>
+      </c>
+      <c r="I61" t="s">
+        <v>310</v>
+      </c>
+      <c r="J61" t="s">
+        <v>400</v>
+      </c>
+      <c r="K61" t="s">
+        <v>401</v>
+      </c>
+      <c r="L61">
+        <v>45.728460900000002</v>
+      </c>
+      <c r="M61">
+        <v>1.7535144</v>
+      </c>
+      <c r="N61">
+        <v>2009</v>
+      </c>
+      <c r="O61">
+        <v>5</v>
+      </c>
+      <c r="P61">
+        <v>13</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>35</v>
+      </c>
+      <c r="V61">
+        <v>1</v>
+      </c>
+      <c r="W61" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="X61" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="Y61" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" t="s">
+        <v>28</v>
+      </c>
+      <c r="F62" t="s">
+        <v>29</v>
+      </c>
+      <c r="G62" t="s">
+        <v>61</v>
+      </c>
+      <c r="H62" t="s">
+        <v>404</v>
+      </c>
+      <c r="I62" t="s">
+        <v>405</v>
+      </c>
+      <c r="J62" t="s">
+        <v>406</v>
+      </c>
+      <c r="K62" t="s">
+        <v>407</v>
+      </c>
+      <c r="L62">
+        <v>48.191289300000001</v>
+      </c>
+      <c r="M62">
+        <v>6.4550101</v>
+      </c>
+      <c r="N62">
+        <v>2009</v>
+      </c>
+      <c r="O62">
+        <v>5</v>
+      </c>
+      <c r="P62">
+        <v>13</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>35</v>
+      </c>
+      <c r="V62">
+        <v>1</v>
+      </c>
+      <c r="W62" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="X62" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="Y62" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B63" t="s">
+        <v>114</v>
+      </c>
+      <c r="C63" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" t="s">
+        <v>28</v>
+      </c>
+      <c r="F63" t="s">
+        <v>29</v>
+      </c>
+      <c r="G63" t="s">
+        <v>30</v>
+      </c>
+      <c r="H63" t="s">
+        <v>138</v>
+      </c>
+      <c r="I63" t="s">
+        <v>410</v>
+      </c>
+      <c r="J63" t="s">
+        <v>411</v>
+      </c>
+      <c r="K63" t="s">
+        <v>412</v>
+      </c>
+      <c r="L63">
+        <v>48.694233799999999</v>
+      </c>
+      <c r="M63">
+        <v>2.2833993000000001</v>
+      </c>
+      <c r="N63">
+        <v>2008</v>
+      </c>
+      <c r="O63">
+        <v>7</v>
+      </c>
+      <c r="P63">
+        <v>6</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>35</v>
+      </c>
+      <c r="V63">
+        <v>1</v>
+      </c>
+      <c r="W63" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="X63" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="Y63" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="64" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
+        <v>114</v>
+      </c>
+      <c r="C64" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" t="s">
+        <v>28</v>
+      </c>
+      <c r="F64" t="s">
+        <v>29</v>
+      </c>
+      <c r="G64" t="s">
+        <v>30</v>
+      </c>
+      <c r="H64" t="s">
+        <v>31</v>
+      </c>
+      <c r="I64" t="s">
+        <v>416</v>
+      </c>
+      <c r="J64" t="s">
+        <v>417</v>
+      </c>
+      <c r="K64" t="s">
+        <v>418</v>
+      </c>
+      <c r="L64">
+        <v>48.948163299999997</v>
+      </c>
+      <c r="M64">
+        <v>2.5321153000000001</v>
+      </c>
+      <c r="N64">
+        <v>2008</v>
+      </c>
+      <c r="O64">
+        <v>8</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>47</v>
+      </c>
+      <c r="V64">
+        <v>1</v>
+      </c>
+      <c r="W64" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="X64" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="Y64" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="65" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" t="s">
+        <v>26</v>
+      </c>
+      <c r="D65" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" t="s">
+        <v>28</v>
+      </c>
+      <c r="F65" t="s">
+        <v>29</v>
+      </c>
+      <c r="G65" t="s">
+        <v>30</v>
+      </c>
+      <c r="H65" t="s">
+        <v>31</v>
+      </c>
+      <c r="I65" t="s">
+        <v>32</v>
+      </c>
+      <c r="J65" t="s">
+        <v>422</v>
+      </c>
+      <c r="K65" t="s">
+        <v>423</v>
+      </c>
+      <c r="L65">
+        <v>48.956174799999999</v>
+      </c>
+      <c r="M65">
+        <v>2.3085974</v>
+      </c>
+      <c r="N65">
+        <v>2008</v>
+      </c>
+      <c r="O65">
+        <v>4</v>
+      </c>
+      <c r="P65">
+        <v>11</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>35</v>
+      </c>
+      <c r="V65">
+        <v>1</v>
+      </c>
+      <c r="W65" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="X65" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="Y65" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="66" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66" t="s">
+        <v>26</v>
+      </c>
+      <c r="D66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E66" t="s">
+        <v>28</v>
+      </c>
+      <c r="F66" t="s">
+        <v>29</v>
+      </c>
+      <c r="G66" t="s">
+        <v>30</v>
+      </c>
+      <c r="H66" t="s">
+        <v>144</v>
+      </c>
+      <c r="I66" t="s">
+        <v>427</v>
+      </c>
+      <c r="J66" t="s">
+        <v>428</v>
+      </c>
+      <c r="K66" t="s">
+        <v>429</v>
+      </c>
+      <c r="L66">
+        <v>48.809092499999998</v>
+      </c>
+      <c r="M66">
+        <v>2.5482450000000001</v>
+      </c>
+      <c r="N66">
+        <v>2008</v>
+      </c>
+      <c r="O66">
+        <v>9</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>47</v>
+      </c>
+      <c r="V66">
+        <v>1</v>
+      </c>
+      <c r="W66" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="X66" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="Y66" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>114</v>
+      </c>
+      <c r="C67" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67" t="s">
+        <v>27</v>
+      </c>
+      <c r="E67" t="s">
+        <v>28</v>
+      </c>
+      <c r="F67" t="s">
+        <v>29</v>
+      </c>
+      <c r="G67" t="s">
+        <v>30</v>
+      </c>
+      <c r="H67" t="s">
+        <v>432</v>
+      </c>
+      <c r="I67" t="s">
+        <v>433</v>
+      </c>
+      <c r="J67" t="s">
+        <v>434</v>
+      </c>
+      <c r="K67" t="s">
+        <v>435</v>
+      </c>
+      <c r="L67">
+        <v>49.01999</v>
+      </c>
+      <c r="M67">
+        <v>2.2229899999999998</v>
+      </c>
+      <c r="N67">
+        <v>2008</v>
+      </c>
+      <c r="O67">
+        <v>7</v>
+      </c>
+      <c r="P67">
+        <v>1</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>35</v>
+      </c>
+      <c r="V67">
+        <v>1</v>
+      </c>
+      <c r="W67" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="X67" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="Y67" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="68" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>439</v>
+      </c>
+      <c r="C68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68" t="s">
+        <v>28</v>
+      </c>
+      <c r="F68" t="s">
+        <v>29</v>
+      </c>
+      <c r="G68" t="s">
+        <v>61</v>
+      </c>
+      <c r="H68" t="s">
+        <v>62</v>
+      </c>
+      <c r="I68" t="s">
+        <v>440</v>
+      </c>
+      <c r="K68" t="s">
+        <v>441</v>
+      </c>
+      <c r="L68">
+        <v>49.284970100000002</v>
+      </c>
+      <c r="M68">
+        <v>4.0209687000000001</v>
+      </c>
+      <c r="N68">
+        <v>2009</v>
+      </c>
+      <c r="O68">
+        <v>5</v>
+      </c>
+      <c r="P68">
+        <v>13</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>35</v>
+      </c>
+      <c r="V68">
+        <v>1</v>
+      </c>
+      <c r="W68" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="X68" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="Y68" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="69" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>114</v>
+      </c>
+      <c r="C69" t="s">
+        <v>26</v>
+      </c>
+      <c r="D69" t="s">
+        <v>27</v>
+      </c>
+      <c r="E69" t="s">
+        <v>28</v>
+      </c>
+      <c r="F69" t="s">
+        <v>29</v>
+      </c>
+      <c r="G69" t="s">
+        <v>77</v>
+      </c>
+      <c r="H69" t="s">
+        <v>94</v>
+      </c>
+      <c r="I69" t="s">
+        <v>222</v>
+      </c>
+      <c r="J69" t="s">
+        <v>445</v>
+      </c>
+      <c r="K69" t="s">
+        <v>446</v>
+      </c>
+      <c r="L69">
+        <v>43.330027999999999</v>
+      </c>
+      <c r="M69">
+        <v>5.3920328</v>
+      </c>
+      <c r="N69">
+        <v>2008</v>
+      </c>
+      <c r="O69">
+        <v>8</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>47</v>
+      </c>
+      <c r="V69">
+        <v>1</v>
+      </c>
+      <c r="W69" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="X69" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="Y69" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>114</v>
+      </c>
+      <c r="C70" t="s">
+        <v>26</v>
+      </c>
+      <c r="D70" t="s">
+        <v>27</v>
+      </c>
+      <c r="E70" t="s">
+        <v>28</v>
+      </c>
+      <c r="F70" t="s">
+        <v>29</v>
+      </c>
+      <c r="G70" t="s">
+        <v>77</v>
+      </c>
+      <c r="H70" t="s">
+        <v>94</v>
+      </c>
+      <c r="I70" t="s">
+        <v>222</v>
+      </c>
+      <c r="J70" t="s">
+        <v>449</v>
+      </c>
+      <c r="K70" s="3">
+        <v>13600</v>
+      </c>
+      <c r="L70">
+        <v>43.184150000000002</v>
+      </c>
+      <c r="M70">
+        <v>5.6063099999999997</v>
+      </c>
+      <c r="N70">
+        <v>2008</v>
+      </c>
+      <c r="O70">
+        <v>7</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>47</v>
+      </c>
+      <c r="V70">
+        <v>1</v>
+      </c>
+      <c r="W70" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="X70" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="Y70" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
+        <v>452</v>
+      </c>
+      <c r="C71" t="s">
+        <v>453</v>
+      </c>
+      <c r="D71" t="s">
+        <v>27</v>
+      </c>
+      <c r="E71" t="s">
+        <v>28</v>
+      </c>
+      <c r="F71" t="s">
+        <v>29</v>
+      </c>
+      <c r="G71" t="s">
+        <v>77</v>
+      </c>
+      <c r="H71" t="s">
+        <v>94</v>
+      </c>
+      <c r="I71" t="s">
+        <v>222</v>
+      </c>
+      <c r="J71" t="s">
+        <v>454</v>
+      </c>
+      <c r="K71" s="3">
+        <v>13240</v>
+      </c>
+      <c r="L71">
+        <v>43.405749999999998</v>
+      </c>
+      <c r="M71">
+        <v>5.3717800000000002</v>
+      </c>
+      <c r="N71">
+        <v>2008</v>
+      </c>
+      <c r="O71">
+        <v>4</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>47</v>
+      </c>
+      <c r="R71" t="s">
+        <v>455</v>
+      </c>
+      <c r="S71" t="s">
+        <v>37</v>
+      </c>
+      <c r="V71">
+        <v>1</v>
+      </c>
+      <c r="W71" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="X71" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="Y71" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>458</v>
+      </c>
+      <c r="C72" t="s">
+        <v>26</v>
+      </c>
+      <c r="D72" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" t="s">
+        <v>28</v>
+      </c>
+      <c r="F72" t="s">
+        <v>29</v>
+      </c>
+      <c r="G72" t="s">
+        <v>86</v>
+      </c>
+      <c r="H72" t="s">
+        <v>87</v>
+      </c>
+      <c r="I72" t="s">
+        <v>88</v>
+      </c>
+      <c r="K72" t="s">
+        <v>459</v>
+      </c>
+      <c r="L72">
+        <v>46.343850000000003</v>
+      </c>
+      <c r="M72">
+        <v>2.6025999999999998</v>
+      </c>
+      <c r="N72">
+        <v>2009</v>
+      </c>
+      <c r="O72">
+        <v>5</v>
+      </c>
+      <c r="P72">
+        <v>13</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>35</v>
+      </c>
+      <c r="V72">
+        <v>1</v>
+      </c>
+      <c r="W72" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="X72" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="Y72" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="73" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
+        <v>463</v>
+      </c>
+      <c r="C73" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" t="s">
+        <v>27</v>
+      </c>
+      <c r="E73" t="s">
+        <v>28</v>
+      </c>
+      <c r="F73" t="s">
+        <v>29</v>
+      </c>
+      <c r="G73" t="s">
+        <v>86</v>
+      </c>
+      <c r="H73" t="s">
+        <v>87</v>
+      </c>
+      <c r="I73" t="s">
+        <v>88</v>
+      </c>
+      <c r="J73" t="s">
+        <v>464</v>
+      </c>
+      <c r="K73" t="s">
+        <v>465</v>
+      </c>
+      <c r="L73">
+        <v>46.368654100000001</v>
+      </c>
+      <c r="M73">
+        <v>2.5342144000000002</v>
+      </c>
+      <c r="N73">
+        <v>2009</v>
+      </c>
+      <c r="O73">
+        <v>5</v>
+      </c>
+      <c r="P73">
+        <v>13</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>35</v>
+      </c>
+      <c r="V73">
+        <v>1</v>
+      </c>
+      <c r="W73" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="X73" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="Y73" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
+        <v>463</v>
+      </c>
+      <c r="C74" t="s">
+        <v>26</v>
+      </c>
+      <c r="D74" t="s">
+        <v>27</v>
+      </c>
+      <c r="E74" t="s">
+        <v>28</v>
+      </c>
+      <c r="F74" t="s">
+        <v>29</v>
+      </c>
+      <c r="G74" t="s">
+        <v>77</v>
+      </c>
+      <c r="H74" t="s">
+        <v>94</v>
+      </c>
+      <c r="I74" t="s">
+        <v>95</v>
+      </c>
+      <c r="J74" t="s">
+        <v>468</v>
+      </c>
+      <c r="K74" t="s">
+        <v>469</v>
+      </c>
+      <c r="L74">
+        <v>43.460058799999999</v>
+      </c>
+      <c r="M74">
+        <v>5.0189871999999998</v>
+      </c>
+      <c r="N74">
+        <v>2009</v>
+      </c>
+      <c r="O74">
+        <v>5</v>
+      </c>
+      <c r="P74">
+        <v>13</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>35</v>
+      </c>
+      <c r="V74">
+        <v>1</v>
+      </c>
+      <c r="W74" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="X74" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="Y74" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
+        <v>463</v>
+      </c>
+      <c r="C75" t="s">
+        <v>26</v>
+      </c>
+      <c r="D75" t="s">
+        <v>27</v>
+      </c>
+      <c r="E75" t="s">
+        <v>28</v>
+      </c>
+      <c r="F75" t="s">
+        <v>29</v>
+      </c>
+      <c r="G75" t="s">
+        <v>130</v>
+      </c>
+      <c r="H75" t="s">
+        <v>472</v>
+      </c>
+      <c r="I75" t="s">
+        <v>473</v>
+      </c>
+      <c r="J75" t="s">
+        <v>474</v>
+      </c>
+      <c r="K75" t="s">
+        <v>475</v>
+      </c>
+      <c r="L75">
+        <v>49.006300500000002</v>
+      </c>
+      <c r="M75">
+        <v>1.1450992</v>
+      </c>
+      <c r="N75">
+        <v>2008</v>
+      </c>
+      <c r="O75">
+        <v>4</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>47</v>
+      </c>
+      <c r="V75">
+        <v>1</v>
+      </c>
+      <c r="W75" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="X75" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="Y75" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>478</v>
+      </c>
+      <c r="C76" t="s">
+        <v>26</v>
+      </c>
+      <c r="D76" t="s">
+        <v>27</v>
+      </c>
+      <c r="E76" t="s">
+        <v>28</v>
+      </c>
+      <c r="F76" t="s">
+        <v>29</v>
+      </c>
+      <c r="G76" t="s">
+        <v>100</v>
+      </c>
+      <c r="H76" t="s">
+        <v>101</v>
+      </c>
+      <c r="I76" t="s">
+        <v>479</v>
+      </c>
+      <c r="J76" t="s">
+        <v>480</v>
+      </c>
+      <c r="K76" s="3">
+        <v>29000</v>
+      </c>
+      <c r="L76">
+        <v>48.00338</v>
+      </c>
+      <c r="M76">
+        <v>-4.0836399999999999</v>
+      </c>
+      <c r="N76">
+        <v>2008</v>
+      </c>
+      <c r="O76">
+        <v>9</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>47</v>
+      </c>
+      <c r="V76">
+        <v>1</v>
+      </c>
+      <c r="W76" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="X76" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="Y76" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="77" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
+        <v>463</v>
+      </c>
+      <c r="C77" t="s">
+        <v>26</v>
+      </c>
+      <c r="D77" t="s">
+        <v>27</v>
+      </c>
+      <c r="E77" t="s">
+        <v>28</v>
+      </c>
+      <c r="F77" t="s">
+        <v>29</v>
+      </c>
+      <c r="G77" t="s">
+        <v>123</v>
+      </c>
+      <c r="H77" t="s">
+        <v>315</v>
+      </c>
+      <c r="I77" t="s">
+        <v>484</v>
+      </c>
+      <c r="K77" t="s">
+        <v>485</v>
+      </c>
+      <c r="L77">
+        <v>50.289467399999999</v>
+      </c>
+      <c r="M77">
+        <v>2.7599556999999999</v>
+      </c>
+      <c r="N77">
+        <v>2009</v>
+      </c>
+      <c r="O77">
+        <v>5</v>
+      </c>
+      <c r="P77">
+        <v>13</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>35</v>
+      </c>
+      <c r="V77">
+        <v>1</v>
+      </c>
+      <c r="W77" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="X77" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="Y77" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="78" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
+        <v>488</v>
+      </c>
+      <c r="C78" t="s">
+        <v>26</v>
+      </c>
+      <c r="D78" t="s">
+        <v>27</v>
+      </c>
+      <c r="E78" t="s">
+        <v>28</v>
+      </c>
+      <c r="F78" t="s">
+        <v>29</v>
+      </c>
+      <c r="G78" t="s">
+        <v>77</v>
+      </c>
+      <c r="H78" t="s">
+        <v>94</v>
+      </c>
+      <c r="I78" t="s">
+        <v>489</v>
+      </c>
+      <c r="J78" t="s">
+        <v>490</v>
+      </c>
+      <c r="K78" t="s">
+        <v>491</v>
+      </c>
+      <c r="L78">
+        <v>43.435283300000002</v>
+      </c>
+      <c r="M78">
+        <v>5.5416334999999997</v>
+      </c>
+      <c r="N78">
+        <v>2009</v>
+      </c>
+      <c r="O78">
+        <v>5</v>
+      </c>
+      <c r="P78">
+        <v>13</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>35</v>
+      </c>
+      <c r="V78">
+        <v>1</v>
+      </c>
+      <c r="W78" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="X78" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="Y78" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B79" t="s">
+        <v>60</v>
+      </c>
+      <c r="C79" t="s">
+        <v>26</v>
+      </c>
+      <c r="D79" t="s">
+        <v>27</v>
+      </c>
+      <c r="E79" t="s">
+        <v>28</v>
+      </c>
+      <c r="F79" t="s">
+        <v>29</v>
+      </c>
+      <c r="G79" t="s">
+        <v>130</v>
+      </c>
+      <c r="H79" t="s">
+        <v>494</v>
+      </c>
+      <c r="I79" t="s">
+        <v>495</v>
+      </c>
+      <c r="J79" t="s">
+        <v>496</v>
+      </c>
+      <c r="K79" t="s">
+        <v>497</v>
+      </c>
+      <c r="L79">
+        <v>49.2286584</v>
+      </c>
+      <c r="M79">
+        <v>-0.3017107</v>
+      </c>
+      <c r="N79">
+        <v>2009</v>
+      </c>
+      <c r="O79">
+        <v>5</v>
+      </c>
+      <c r="P79">
+        <v>13</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>35</v>
+      </c>
+      <c r="R79" t="s">
+        <v>498</v>
+      </c>
+      <c r="S79" t="s">
+        <v>37</v>
+      </c>
+      <c r="V79">
+        <v>1</v>
+      </c>
+      <c r="W79" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="X79" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="Y79" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
+        <v>488</v>
+      </c>
+      <c r="C80" t="s">
+        <v>26</v>
+      </c>
+      <c r="D80" t="s">
+        <v>27</v>
+      </c>
+      <c r="E80" t="s">
+        <v>28</v>
+      </c>
+      <c r="F80" t="s">
+        <v>29</v>
+      </c>
+      <c r="G80" t="s">
+        <v>42</v>
+      </c>
+      <c r="H80" t="s">
+        <v>501</v>
+      </c>
+      <c r="I80" t="s">
+        <v>502</v>
+      </c>
+      <c r="K80" t="s">
+        <v>503</v>
+      </c>
+      <c r="L80">
+        <v>45.647343800000002</v>
+      </c>
+      <c r="M80">
+        <v>0.16687170000000001</v>
+      </c>
+      <c r="N80">
+        <v>2009</v>
+      </c>
+      <c r="O80">
+        <v>5</v>
+      </c>
+      <c r="P80">
+        <v>13</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>35</v>
+      </c>
+      <c r="R80" t="s">
+        <v>504</v>
+      </c>
+      <c r="S80" t="s">
+        <v>37</v>
+      </c>
+      <c r="V80">
+        <v>1</v>
+      </c>
+      <c r="W80" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="X80" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="Y80" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B81" t="s">
+        <v>507</v>
+      </c>
+      <c r="C81" t="s">
+        <v>26</v>
+      </c>
+      <c r="D81" t="s">
+        <v>27</v>
+      </c>
+      <c r="E81" t="s">
+        <v>28</v>
+      </c>
+      <c r="F81" t="s">
+        <v>29</v>
+      </c>
+      <c r="G81" t="s">
+        <v>51</v>
+      </c>
+      <c r="H81" t="s">
+        <v>227</v>
+      </c>
+      <c r="I81" t="s">
+        <v>508</v>
+      </c>
+      <c r="J81" t="s">
+        <v>509</v>
+      </c>
+      <c r="K81" t="s">
+        <v>510</v>
+      </c>
+      <c r="L81">
+        <v>47.226520000000001</v>
+      </c>
+      <c r="M81">
+        <v>2.0865999999999998</v>
+      </c>
+      <c r="N81">
+        <v>2009</v>
+      </c>
+      <c r="O81">
+        <v>5</v>
+      </c>
+      <c r="P81">
+        <v>13</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>35</v>
+      </c>
+      <c r="V81">
+        <v>1</v>
+      </c>
+      <c r="W81" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="X81" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="Y81" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="82" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B82" t="s">
+        <v>488</v>
+      </c>
+      <c r="C82" t="s">
+        <v>26</v>
+      </c>
+      <c r="D82" t="s">
+        <v>27</v>
+      </c>
+      <c r="E82" t="s">
+        <v>28</v>
+      </c>
+      <c r="F82" t="s">
+        <v>29</v>
+      </c>
+      <c r="G82" t="s">
+        <v>234</v>
+      </c>
+      <c r="H82" t="s">
+        <v>235</v>
+      </c>
+      <c r="I82" t="s">
+        <v>236</v>
+      </c>
+      <c r="J82" t="s">
+        <v>514</v>
+      </c>
+      <c r="K82" t="s">
+        <v>238</v>
+      </c>
+      <c r="L82">
+        <v>47.303229999999999</v>
+      </c>
+      <c r="M82">
+        <v>5.1194499999999996</v>
+      </c>
+      <c r="N82">
+        <v>2008</v>
+      </c>
+      <c r="O82">
+        <v>7</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>47</v>
+      </c>
+      <c r="V82">
+        <v>1</v>
+      </c>
+      <c r="W82" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="X82" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="Y82" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B83" t="s">
+        <v>488</v>
+      </c>
+      <c r="C83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D83" t="s">
+        <v>27</v>
+      </c>
+      <c r="E83" t="s">
+        <v>28</v>
+      </c>
+      <c r="F83" t="s">
+        <v>29</v>
+      </c>
+      <c r="G83" t="s">
+        <v>234</v>
+      </c>
+      <c r="H83" t="s">
+        <v>517</v>
+      </c>
+      <c r="I83" t="s">
+        <v>518</v>
+      </c>
+      <c r="J83" t="s">
+        <v>519</v>
+      </c>
+      <c r="K83" t="s">
+        <v>520</v>
+      </c>
+      <c r="L83">
+        <v>47.219720000000002</v>
+      </c>
+      <c r="M83">
+        <v>5.97316</v>
+      </c>
+      <c r="N83">
+        <v>2009</v>
+      </c>
+      <c r="O83">
+        <v>5</v>
+      </c>
+      <c r="P83">
+        <v>13</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>35</v>
+      </c>
+      <c r="V83">
+        <v>1</v>
+      </c>
+      <c r="W83" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="X83" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="Y83" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="84" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B84" t="s">
+        <v>488</v>
+      </c>
+      <c r="C84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D84" t="s">
+        <v>27</v>
+      </c>
+      <c r="E84" t="s">
+        <v>28</v>
+      </c>
+      <c r="F84" t="s">
+        <v>29</v>
+      </c>
+      <c r="G84" t="s">
+        <v>100</v>
+      </c>
+      <c r="H84" t="s">
+        <v>101</v>
+      </c>
+      <c r="I84" t="s">
+        <v>479</v>
+      </c>
+      <c r="J84" t="s">
+        <v>523</v>
+      </c>
+      <c r="K84" t="s">
+        <v>524</v>
+      </c>
+      <c r="L84">
+        <v>48.095790000000001</v>
+      </c>
+      <c r="M84">
+        <v>-4.3446100000000003</v>
+      </c>
+      <c r="N84">
+        <v>2009</v>
+      </c>
+      <c r="O84">
+        <v>5</v>
+      </c>
+      <c r="P84">
+        <v>13</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>35</v>
+      </c>
+      <c r="T84" t="s">
+        <v>533</v>
+      </c>
+      <c r="V84">
+        <v>1</v>
+      </c>
+      <c r="W84" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="X84" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="Y84" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="85" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B85" t="s">
+        <v>488</v>
+      </c>
+      <c r="C85" t="s">
+        <v>26</v>
+      </c>
+      <c r="D85" t="s">
+        <v>27</v>
+      </c>
+      <c r="E85" t="s">
+        <v>28</v>
+      </c>
+      <c r="F85" t="s">
+        <v>29</v>
+      </c>
+      <c r="G85" t="s">
+        <v>42</v>
+      </c>
+      <c r="H85" t="s">
+        <v>43</v>
+      </c>
+      <c r="I85" t="s">
+        <v>528</v>
+      </c>
+      <c r="J85" t="s">
+        <v>529</v>
+      </c>
+      <c r="K85" t="s">
+        <v>530</v>
+      </c>
+      <c r="L85">
+        <v>44.549566200000001</v>
+      </c>
+      <c r="M85">
+        <v>-0.24376149999999999</v>
+      </c>
+      <c r="N85">
+        <v>2009</v>
+      </c>
+      <c r="O85">
+        <v>5</v>
+      </c>
+      <c r="P85">
+        <v>13</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>35</v>
+      </c>
+      <c r="V85">
+        <v>1</v>
+      </c>
+      <c r="W85" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="X85" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="Y85" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -4076,6 +7538,137 @@
     <hyperlink ref="X39" r:id="rId118" xr:uid="{F8E62B96-C5F3-420D-860B-884BB0250FFA}"/>
     <hyperlink ref="X40" r:id="rId119" xr:uid="{377C01A0-2B46-48AE-98E6-E95CA909B977}"/>
     <hyperlink ref="X41" r:id="rId120" xr:uid="{E8F7FDEE-C493-4B87-941A-CF6401BE2758}"/>
+    <hyperlink ref="W42" r:id="rId121" xr:uid="{9E292334-DC68-433E-9DBD-D01EBE1A0BF8}"/>
+    <hyperlink ref="Y42" r:id="rId122" xr:uid="{11ABC610-0092-4FF1-9B86-D4C011A00674}"/>
+    <hyperlink ref="W43" r:id="rId123" xr:uid="{9130981A-925E-4E17-9291-056E223BEBDA}"/>
+    <hyperlink ref="Y43" r:id="rId124" xr:uid="{0C26D97B-08D1-4D33-8AAF-4BE9AE055E64}"/>
+    <hyperlink ref="W44" r:id="rId125" xr:uid="{D837C679-72DB-402B-B88F-D6649A6C8683}"/>
+    <hyperlink ref="Y44" r:id="rId126" xr:uid="{0C4B6637-1ACE-4C9D-82DD-8022B4DD80DC}"/>
+    <hyperlink ref="W45" r:id="rId127" xr:uid="{0544AAFB-4336-4032-86AA-C2B3D23C26FD}"/>
+    <hyperlink ref="Y45" r:id="rId128" xr:uid="{35583C0D-00D9-448B-B0B2-5B659475D045}"/>
+    <hyperlink ref="W46" r:id="rId129" xr:uid="{2F51F27D-4E15-43BC-AE50-0473152645C9}"/>
+    <hyperlink ref="Y46" r:id="rId130" xr:uid="{7BF02CE2-25AE-4960-97FE-ED24DFF24693}"/>
+    <hyperlink ref="W47" r:id="rId131" xr:uid="{3CCFD53D-8AE7-405F-9669-81353AA2723D}"/>
+    <hyperlink ref="Y47" r:id="rId132" xr:uid="{238D937B-6EB4-4318-9430-25AAAED654C0}"/>
+    <hyperlink ref="W48" r:id="rId133" xr:uid="{56F5A8A9-2D12-4452-B828-F447A1CD6D81}"/>
+    <hyperlink ref="Y48" r:id="rId134" xr:uid="{EA5BAA63-8E91-4469-9F7F-D27CDA33FB9F}"/>
+    <hyperlink ref="W49" r:id="rId135" xr:uid="{0EFA98FA-CE34-4E02-951D-18C0354233DB}"/>
+    <hyperlink ref="Y49" r:id="rId136" xr:uid="{AE8FF7F2-E9F0-40BA-8100-51623E517616}"/>
+    <hyperlink ref="W50" r:id="rId137" xr:uid="{E534F51D-62E8-4326-AF55-6D5C88B178D7}"/>
+    <hyperlink ref="Y50" r:id="rId138" xr:uid="{64547C0F-195F-4FB9-8F0C-B1D6CDB08A6E}"/>
+    <hyperlink ref="W51" r:id="rId139" xr:uid="{FDD152F9-259B-45B9-9CE5-99C47A3F47A6}"/>
+    <hyperlink ref="Y51" r:id="rId140" xr:uid="{F6211230-8B62-44D4-90D6-FF7A7676A5AB}"/>
+    <hyperlink ref="W52" r:id="rId141" xr:uid="{99D3A98C-37BC-4923-A169-07C56E8F1796}"/>
+    <hyperlink ref="Y52" r:id="rId142" xr:uid="{2FE25CA0-C46E-40CA-9D81-5D4A6041D937}"/>
+    <hyperlink ref="W53" r:id="rId143" xr:uid="{948533D0-5CE4-4C40-B025-17387D64DB3A}"/>
+    <hyperlink ref="Y53" r:id="rId144" xr:uid="{C4D897D5-16ED-4329-8473-D128435268DC}"/>
+    <hyperlink ref="W54" r:id="rId145" xr:uid="{7C3BA1C2-3161-459A-A86E-C6545CDDADCE}"/>
+    <hyperlink ref="Y54" r:id="rId146" xr:uid="{7A9D0FD2-A1D3-4010-A140-DA67D0FEA215}"/>
+    <hyperlink ref="W55" r:id="rId147" xr:uid="{150508DA-1459-4151-A1F2-2BBFE57BC53A}"/>
+    <hyperlink ref="Y55" r:id="rId148" xr:uid="{9CFA708E-2F7B-4544-A436-88CD813F045E}"/>
+    <hyperlink ref="W58" r:id="rId149" xr:uid="{9A8079BD-DD41-41A2-8814-D32D385CE79B}"/>
+    <hyperlink ref="W59" r:id="rId150" xr:uid="{E24CC28D-5979-46AE-A57F-953C1D59C656}"/>
+    <hyperlink ref="Y59" r:id="rId151" xr:uid="{A49E730D-FA77-41AD-9E97-96F31AA3A850}"/>
+    <hyperlink ref="W60" r:id="rId152" xr:uid="{6AE593F8-C0AC-434E-98F7-51534773CC40}"/>
+    <hyperlink ref="Y60" r:id="rId153" xr:uid="{EA6EB665-4003-487E-87E3-5471CD9E809F}"/>
+    <hyperlink ref="W61" r:id="rId154" xr:uid="{13A0413A-89D1-4D6F-B257-B16F717B187C}"/>
+    <hyperlink ref="Y61" r:id="rId155" xr:uid="{243CFAE6-60AC-4B7D-8E3C-297C6219A911}"/>
+    <hyperlink ref="W62" r:id="rId156" xr:uid="{34FFB234-AA9E-4BCC-A580-6C76F4AADF80}"/>
+    <hyperlink ref="Y62" r:id="rId157" xr:uid="{411744C3-C770-4F21-BB90-F41C733E8C05}"/>
+    <hyperlink ref="W63" r:id="rId158" xr:uid="{6962A861-E71F-46B6-9B7B-25846195685A}"/>
+    <hyperlink ref="Y63" r:id="rId159" xr:uid="{C1995EAC-0A24-4AAE-B9B0-169DFD14A256}"/>
+    <hyperlink ref="X42" r:id="rId160" xr:uid="{6D8B8371-AADA-4439-BFF6-B8876A075D44}"/>
+    <hyperlink ref="X43" r:id="rId161" xr:uid="{BD7F5AF4-A2FE-4216-AE8D-C1784E371BDC}"/>
+    <hyperlink ref="X44" r:id="rId162" xr:uid="{307E9FF0-06D9-4DDA-97D4-80A873E127F5}"/>
+    <hyperlink ref="X45" r:id="rId163" xr:uid="{4DE865F7-6526-490E-9114-A6CEFBFE8199}"/>
+    <hyperlink ref="X46" r:id="rId164" xr:uid="{EE8959B2-CA9B-47BD-96B0-E42058826757}"/>
+    <hyperlink ref="X47" r:id="rId165" xr:uid="{65655281-580C-45FF-BFEE-D47CEB502C69}"/>
+    <hyperlink ref="X48" r:id="rId166" xr:uid="{B4F80422-51CC-4250-AB52-A700DF07B021}"/>
+    <hyperlink ref="X49" r:id="rId167" xr:uid="{9C638F6E-4AEF-4EAC-A2BE-33F45DE0390F}"/>
+    <hyperlink ref="X50" r:id="rId168" xr:uid="{30318520-BAB0-4013-96DE-F718D09867C2}"/>
+    <hyperlink ref="X51" r:id="rId169" xr:uid="{BEC40995-FABD-4B4D-A41E-13BB1425B849}"/>
+    <hyperlink ref="X52" r:id="rId170" xr:uid="{B768E462-46E3-47DA-84F7-C140FEBBCE9D}"/>
+    <hyperlink ref="X53" r:id="rId171" xr:uid="{FDE85BF9-7C67-4565-A002-C39149AF33BC}"/>
+    <hyperlink ref="X54" r:id="rId172" xr:uid="{FF22C78A-61BA-40FF-89CC-7223881FA8D1}"/>
+    <hyperlink ref="X55" r:id="rId173" xr:uid="{E5C10D66-24ED-4C85-8BEC-BF764F161565}"/>
+    <hyperlink ref="W56" r:id="rId174" xr:uid="{134ED401-18F8-4226-B2B8-CEA79C2F3E90}"/>
+    <hyperlink ref="X56" r:id="rId175" xr:uid="{01FC26BE-8367-4C14-835A-168D38BEB78F}"/>
+    <hyperlink ref="Y58" r:id="rId176" xr:uid="{DB8A8E68-8398-4463-A747-382BACD77ED6}"/>
+    <hyperlink ref="Y56" r:id="rId177" xr:uid="{A10AD225-511C-4B53-89B9-B5C7CCC420D6}"/>
+    <hyperlink ref="W57" r:id="rId178" xr:uid="{E9C9E73A-4D95-4ABF-98B2-3E9C18CE40B4}"/>
+    <hyperlink ref="X57" r:id="rId179" xr:uid="{C8E1C5EE-3AFB-4693-9C85-B9FA15BDE981}"/>
+    <hyperlink ref="Y57" r:id="rId180" xr:uid="{0A9C5B6E-1ED6-4CB8-B1E7-D041698C913A}"/>
+    <hyperlink ref="X58" r:id="rId181" xr:uid="{8E2C2C4B-0091-469F-A59B-1A2C3001DC30}"/>
+    <hyperlink ref="X59" r:id="rId182" xr:uid="{B2F0DC39-77CE-45F8-BA94-6324EDCAD914}"/>
+    <hyperlink ref="X60" r:id="rId183" xr:uid="{7C6FCEA2-7074-42D2-A1B7-40B9E8E3B476}"/>
+    <hyperlink ref="X61" r:id="rId184" xr:uid="{955C3D04-C684-4A65-B782-B1EDE3332D87}"/>
+    <hyperlink ref="X62" r:id="rId185" xr:uid="{6B798524-6E91-49D5-8D36-70E84CC88A76}"/>
+    <hyperlink ref="X63" r:id="rId186" xr:uid="{E99B9ACF-3A37-4C1F-BDDF-0EA266E6F1F5}"/>
+    <hyperlink ref="W64" r:id="rId187" xr:uid="{D77B3F7F-CD74-4DC3-A897-DFAB7569F353}"/>
+    <hyperlink ref="Y64" r:id="rId188" xr:uid="{15233F54-E0D9-4404-92B7-0CBD0E44B771}"/>
+    <hyperlink ref="W65" r:id="rId189" xr:uid="{8B9A2E5F-7455-45E3-B095-9BAA8E9F7B14}"/>
+    <hyperlink ref="Y65" r:id="rId190" xr:uid="{3F4B9BBE-E42E-4588-83AF-CD627B63AD9A}"/>
+    <hyperlink ref="W66" r:id="rId191" xr:uid="{05728CFC-0868-45C0-A178-23AB1156C8A4}"/>
+    <hyperlink ref="Y66" r:id="rId192" xr:uid="{EF95F9C2-B8BF-4DBF-8BB4-C6B0FBF9E1A2}"/>
+    <hyperlink ref="W67" r:id="rId193" xr:uid="{ACEC2B72-8122-42E9-8EB6-AE5A0F79F294}"/>
+    <hyperlink ref="Y67" r:id="rId194" xr:uid="{51775ECD-5A8C-44E1-9E92-894B93DC8D85}"/>
+    <hyperlink ref="W68" r:id="rId195" xr:uid="{833BB07F-85FD-4D11-A394-20406F5344E9}"/>
+    <hyperlink ref="Y68" r:id="rId196" xr:uid="{BDF7C608-20F9-4CE8-A137-E4B07A3C8BD9}"/>
+    <hyperlink ref="W69" r:id="rId197" xr:uid="{E48961FC-15D7-49F7-89A6-A6269854F56B}"/>
+    <hyperlink ref="Y69" r:id="rId198" xr:uid="{1DB259B7-FFDA-4AA7-AFA4-49A945318500}"/>
+    <hyperlink ref="W72" r:id="rId199" xr:uid="{71761368-F870-474E-9CF8-9C5A665A2418}"/>
+    <hyperlink ref="Y72" r:id="rId200" xr:uid="{5B666895-B8F6-4D59-A93C-9EF232E1163B}"/>
+    <hyperlink ref="W73" r:id="rId201" xr:uid="{F53FBE7B-D8BB-4E80-B684-2A64442AA087}"/>
+    <hyperlink ref="Y73" r:id="rId202" xr:uid="{AB734A53-EA58-427F-A4FB-4984D0B26805}"/>
+    <hyperlink ref="W74" r:id="rId203" xr:uid="{F2A1B4A9-7226-43E3-A4CA-F8C8CC9911CB}"/>
+    <hyperlink ref="Y74" r:id="rId204" xr:uid="{EE158BCF-991C-41BA-BF64-37E37283A7C3}"/>
+    <hyperlink ref="W75" r:id="rId205" xr:uid="{C5840CCC-3C87-4460-9F58-CB9A5C880B41}"/>
+    <hyperlink ref="Y75" r:id="rId206" xr:uid="{9967A45D-5BA4-4E1D-B376-9F94EEDDFB1D}"/>
+    <hyperlink ref="W76" r:id="rId207" xr:uid="{A0F24A74-D3C1-4A35-B90C-056D1DE3E0F9}"/>
+    <hyperlink ref="Y76" r:id="rId208" xr:uid="{E586A9C2-F045-444A-8DCA-A521D44B0B67}"/>
+    <hyperlink ref="W77" r:id="rId209" xr:uid="{53C095F8-EFFD-488F-8375-BF066A505370}"/>
+    <hyperlink ref="Y77" r:id="rId210" xr:uid="{BB1EE10A-8AEA-49AA-AC59-EE256098415D}"/>
+    <hyperlink ref="W78" r:id="rId211" xr:uid="{4C564BD7-D101-49B3-AA24-8A00DA386E1D}"/>
+    <hyperlink ref="Y78" r:id="rId212" xr:uid="{2CD8234E-529A-4BDD-8AE6-4FCC9A37AA54}"/>
+    <hyperlink ref="W79" r:id="rId213" xr:uid="{F112753A-658D-480E-8754-7C179A84159F}"/>
+    <hyperlink ref="Y79" r:id="rId214" xr:uid="{8147CFEF-B1A1-458A-8CA6-034553F60929}"/>
+    <hyperlink ref="W80" r:id="rId215" xr:uid="{832B8F29-9401-46B7-98A3-68AF5138FA25}"/>
+    <hyperlink ref="Y80" r:id="rId216" xr:uid="{12C56ADA-09BC-4F69-AD7C-DB29929BC34E}"/>
+    <hyperlink ref="W81" r:id="rId217" xr:uid="{E20A1D17-177C-428C-AAB5-90FE77ED3EAC}"/>
+    <hyperlink ref="Y81" r:id="rId218" xr:uid="{6F6474F8-5944-487E-BC21-EAC8C383274F}"/>
+    <hyperlink ref="Y82" r:id="rId219" xr:uid="{D15BA706-31E0-46DA-BADF-08D95CB05BE9}"/>
+    <hyperlink ref="W83" r:id="rId220" xr:uid="{58BF3D98-EAC0-490B-8067-8005BB75C959}"/>
+    <hyperlink ref="Y83" r:id="rId221" xr:uid="{E9C5787F-7E35-4B72-B3E2-DB4FD615914F}"/>
+    <hyperlink ref="W84" r:id="rId222" xr:uid="{CC0BF2D4-3128-454D-BC41-4B11985480E0}"/>
+    <hyperlink ref="Y84" r:id="rId223" xr:uid="{8625EE15-6CAE-472D-8C38-34E359F4D9D2}"/>
+    <hyperlink ref="W85" r:id="rId224" xr:uid="{9A4566B2-ADB5-4147-B574-8BB51EE86B97}"/>
+    <hyperlink ref="Y85" r:id="rId225" xr:uid="{789AEF6B-1BFE-4B93-881F-0BACA33EA3B4}"/>
+    <hyperlink ref="X64" r:id="rId226" xr:uid="{2BF4B7C5-FDFC-4CF7-BA1A-D1806C08A5EB}"/>
+    <hyperlink ref="X65" r:id="rId227" xr:uid="{EC712B4D-0FAC-44EC-8F12-590EB1BE7260}"/>
+    <hyperlink ref="X66" r:id="rId228" xr:uid="{1572D41D-DCC3-47EA-9507-8B3BD10B4925}"/>
+    <hyperlink ref="X67" r:id="rId229" xr:uid="{9D335920-29BC-4F25-A8F2-63A990A5703C}"/>
+    <hyperlink ref="X68" r:id="rId230" xr:uid="{241555FB-0479-411D-8B62-0B354B95A6BB}"/>
+    <hyperlink ref="X69" r:id="rId231" xr:uid="{50F71871-F759-4D06-B29D-CA0D209FBC30}"/>
+    <hyperlink ref="X72" r:id="rId232" xr:uid="{FA115550-A707-49EF-B5F0-BD42D574CA96}"/>
+    <hyperlink ref="X73" r:id="rId233" xr:uid="{0110267B-78AD-4675-8BFB-429F8BB28E60}"/>
+    <hyperlink ref="X74" r:id="rId234" xr:uid="{AD74E859-819A-4B77-BD9C-B75CEA1A644A}"/>
+    <hyperlink ref="X75" r:id="rId235" xr:uid="{26241A1F-9EEA-4DC4-964C-ACD09E91C176}"/>
+    <hyperlink ref="X76" r:id="rId236" xr:uid="{6F6381A3-70D6-480D-B1C8-6E54C6072273}"/>
+    <hyperlink ref="X77" r:id="rId237" xr:uid="{3B7E446F-97CB-4B2C-AEA0-7B45631F8B36}"/>
+    <hyperlink ref="X78" r:id="rId238" xr:uid="{F1FA924D-728F-465F-9408-B83C2B9CCD0A}"/>
+    <hyperlink ref="X79" r:id="rId239" xr:uid="{A205E7A8-3F89-4549-AA24-7160EE2E9B5B}"/>
+    <hyperlink ref="X80" r:id="rId240" xr:uid="{00076D8D-2C45-49C9-B79E-736C5D586C1B}"/>
+    <hyperlink ref="X81" r:id="rId241" xr:uid="{EBD7B964-9222-4E9C-BB9D-C5E6FEE2DD1A}"/>
+    <hyperlink ref="X83" r:id="rId242" xr:uid="{A065E1C6-953B-41C3-B340-A21DCDE4DE14}"/>
+    <hyperlink ref="X84" r:id="rId243" xr:uid="{3E9A04B1-59FE-4ACA-967D-012FADA0B6AD}"/>
+    <hyperlink ref="X85" r:id="rId244" xr:uid="{D8771BA6-4109-4864-AEF4-74B776C04B50}"/>
+    <hyperlink ref="W70" r:id="rId245" xr:uid="{61D0646A-289D-4D1D-A10D-80701ACC1D4E}"/>
+    <hyperlink ref="X70" r:id="rId246" xr:uid="{CE4A79BE-C8C1-4C95-9981-66D28E11DD07}"/>
+    <hyperlink ref="W71" r:id="rId247" xr:uid="{BBA976D0-5AE5-4D53-95A8-51219C050D8C}"/>
+    <hyperlink ref="X71" r:id="rId248" xr:uid="{85AF8487-ABC6-47AB-83DA-46E63F08C101}"/>
+    <hyperlink ref="Y70:Y71" r:id="rId249" display="http://www.abacq.org/calle/index.php?2009/05/13/349-salvador-allende-en-francia" xr:uid="{73E4C761-1B4A-4CA8-9B8E-32FD173D6D3D}"/>
+    <hyperlink ref="X82" r:id="rId250" xr:uid="{56CE1432-C4F3-42A4-82E0-7F2BFA89CE2D}"/>
+    <hyperlink ref="W82" r:id="rId251" xr:uid="{AE6BFA73-1A9A-4092-A549-43EF6BAF9D95}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
More FR data, work on allende_in_france_paris.py
</commit_message>
<xml_diff>
--- a/a-place-for-salvador-allende/countries/France_all.xlsx
+++ b/a-place-for-salvador-allende/countries/France_all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GoGro\Desktop\Repos\datasets-of-interest\a-place-for-salvador-allende\countries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD82581-7470-4331-8D08-EEDBD0B33562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9BC7BD-DEE6-48FB-B700-15F7A04D87AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13760" xr2:uid="{FB19995C-71E8-4436-B5BB-733167ED68ED}"/>
+    <workbookView xWindow="33480" yWindow="2925" windowWidth="29040" windowHeight="17790" xr2:uid="{FB19995C-71E8-4436-B5BB-733167ED68ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5029" uniqueCount="1886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5358" uniqueCount="2013">
   <si>
     <t>id</t>
   </si>
@@ -5860,6 +5860,433 @@
   </si>
   <si>
     <t>http://www.abacq.org/calle/index.php?2009/05/29/356-paris-francia</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/05/09/348-hendaya-francia</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/04/01/336-villiers-le-bel-francia</t>
+  </si>
+  <si>
+    <t>Complexe sportif Salvador Allende</t>
+  </si>
+  <si>
+    <t>sports center</t>
+  </si>
+  <si>
+    <t>Fontenay-sous-Bois</t>
+  </si>
+  <si>
+    <t>94120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Hommage à Salvador Allende, Président de la République du Chili, de 1970 a 1973, renversé et assassiné lors du coup d'état militaire du 11 septembre 1973. La ville de Fontenay-Sous-Bois a accueilli de nombreux réfugiés Chiliens. Ils y ont apporté leur amitié et leurs talents.
+Le 10 septembre 2003
+Jean-François VOGUET, Maire,
+et la Municipalité"
+</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/767469782</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/ukeGWtHun6iymqxs9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/03/15/334-fontenay-sous-bois-francia</t>
+  </si>
+  <si>
+    <t>Branly - Boissière</t>
+  </si>
+  <si>
+    <t>93100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montreuil 
+Avenue du Président Salvador Allende 
+Président du Gouvernement d'Unité Populaire du Chili 
+Assassiné par les fascistes chiliens le 11 septembre 1973
+</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/23305341</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/7sJXWqpiLZ4RD6Nw7</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/03/05/332-montreuil-francia</t>
+  </si>
+  <si>
+    <t>Athis-Mons</t>
+  </si>
+  <si>
+    <t>91200</t>
+  </si>
+  <si>
+    <t>Athis-Mons 
+Place Salvador Allende 
+1908 - 1973 
+Président du CHILI 
+1970 - 1973</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/40994890</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/Na3P4aHq9yiLgEk5A</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/02/10/317-athis-mons-francia</t>
+  </si>
+  <si>
+    <t>Houilles</t>
+  </si>
+  <si>
+    <t>78800</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/9819823768</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/Sg8AvpNbgE46f7ur6</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/02/10/315-houilles-francia</t>
+  </si>
+  <si>
+    <t>Memorial plate to Salvador Allende</t>
+  </si>
+  <si>
+    <t>memorial plate</t>
+  </si>
+  <si>
+    <t>Orly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je resisterai par tous les moyens et au prix de ma vie pour laisser a l'histoire l'ignominie de ceux qui possedent la force mais non la raison 
+Salvador Allende 
+Président de la République du Chili 
+(1970-1973) 
+La municipalité s'associe aux chiliens de la ville pour rendre hommage à Salvador Allende, assassiné le 11 septembre 1973 
+Gaston Viens, Alcalde, consejero municipal del Val de Marne. El 11 de septiembre 1993
+</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/02/01/309-orly-francia</t>
+  </si>
+  <si>
+    <t>Saint-Jean-de-la-Ruelle</t>
+  </si>
+  <si>
+    <t>"Bientôt s'ouvriront à nouveau les grandes avenues où passera l'homme libre pour construire une société meilleure" 
+Salvador Allende 
+1908 - 1973</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/1026315309</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/fBTkZH7s6KrQJ7kq6</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/01/05/298-saint-jean-de-la-ruelle-francia</t>
+  </si>
+  <si>
+    <t>Collège Salvador Allende</t>
+  </si>
+  <si>
+    <t>Auboué</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/3zfmermPUUvc51v38</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/11/22/288-auboue-francia</t>
+  </si>
+  <si>
+    <t>Esplanade Salvador Allende</t>
+  </si>
+  <si>
+    <t>Una calle del Presidente Salvador Allende en Argenteuil.
+Un golpe militar acaba de derrocar el gobierno legal de unidad popular en Chile.
+Las fuerzas reaccionarias con la ayuda de las compañías multinacionales del cobre y del teléfono, apoyadas por el imperialismo estadounidense violan la legalidad, suprimen las libertades, provocan la guerra civil para reconquistar sus privilegios.
+Una represión sangrienta se abate sobre el movimiento obrero y democrático.
+Las víctimas se cuentan ya por miles.
+Una de las primeras víctimas es el presidente de la República Salvador Allende.
+El Consejo Municipal reunido en sesión pública el 14 de septiembre de 1973 saluda con respeto al militante valiente y decidido, muerto en combate y que perdurará como el símbolo de la Unidad Popular.
+Para perpetuar su memoria y destacar la solidaridad de los habitantes de Argenteuil con el pueblo chileno el consejo municipal, por unanimidad, ha decidido darle el nombre de Presidente Salvador Allende a la nueva vía del centro de la ciudad que unirá la calle de la Libertad con la calle del 8 de Mayo de 1945.</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/316584419</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/DVP1AVQsVz67zDdz5</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/11/05/281-argenteuil-francia</t>
+  </si>
+  <si>
+    <t>Stains</t>
+  </si>
+  <si>
+    <t>93240</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/40282846</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/h4VgpUvRRtWitd58A</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/09/19/269-stains-francia</t>
+  </si>
+  <si>
+    <t>Tremblay-en-France</t>
+  </si>
+  <si>
+    <t>93290</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/31058028</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/fvTx3adReHa2V3cp7</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/09/11/266-tremblay-en-france-francia</t>
+  </si>
+  <si>
+    <t>Carrefour Salvadore-Allende</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/350447942</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/TiW4qj8poxs4G2q17</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/09/08/263-chatenay-malabry-francia</t>
+  </si>
+  <si>
+    <t>Rennes</t>
+  </si>
+  <si>
+    <t>Quartiers Ouest</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/259538397</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/6cQP6jACGTxTEmu1A</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/09/05/258-redon-francia</t>
+  </si>
+  <si>
+    <t>Romainville</t>
+  </si>
+  <si>
+    <t>93230</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/934499545</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/XYtqo4ZR8EGt1Avw9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/09/01/255-romainville-francia</t>
+  </si>
+  <si>
+    <t>Bagnolet</t>
+  </si>
+  <si>
+    <t>93170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le 27 octobre 1973 
+Le conseil municipal a donné a la place de la mairie, le nom de 
+Salvador Allende 
+Président légitime de la République du Chili 
+Assassiné par une junte militaire fasciste 
+</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/relation/11750191</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/PbQmdV5gMPu4E3cQ7</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/08/29/251-bagnolet-francia</t>
+  </si>
+  <si>
+    <t>Carrefour Salvador Allende</t>
+  </si>
+  <si>
+    <t>Les Pavillons-sous-Bois</t>
+  </si>
+  <si>
+    <t>93320</t>
+  </si>
+  <si>
+    <t>Pavillons sous Bois / Livry-Gargan 
+Carrefour Salvador Allende 
+Militant socialiste 
+Président de la république chilienne 
+Assassiné le 11 septembre 1973 
+1908 - 1973</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/149569076</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/pPPGNi9CrVhk3jGp9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/08/27/249-pavillons-sous-bois-livry-gargan-francia</t>
+  </si>
+  <si>
+    <t>Front de Lac - Ormetteau -Port</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/400575973</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/nkUH9F8vK8LTKupt7</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/08/25/247-creteil-francia</t>
+  </si>
+  <si>
+    <t>Guadeloupe</t>
+  </si>
+  <si>
+    <t>Pointe-à-Pitre</t>
+  </si>
+  <si>
+    <t>Port-Louis</t>
+  </si>
+  <si>
+    <t>97117</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/392193473</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/08/25/245-pointe-a-pitre-guadeloupe-francia</t>
+  </si>
+  <si>
+    <t>Villepinte</t>
+  </si>
+  <si>
+    <t>93420</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/48562961</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/gTcdNqgDoCVYNsCn8</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/08/25/244-villepinte-francia</t>
+  </si>
+  <si>
+    <t>Place du Président Salvador Allende</t>
+  </si>
+  <si>
+    <t>Pierrefitte-sur-Seine</t>
+  </si>
+  <si>
+    <t>93380</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/1157193005</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/NRpKMAtM5XYVQeyi6</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/07/24/243-pierrefitte-sur-seine-francia</t>
+  </si>
+  <si>
+    <t>Pantin</t>
+  </si>
+  <si>
+    <t>93500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A la mémoire de 
+Salvador Allende 
+1908 - 1973 
+Président de la République du Chili 
+1970 - 1973
+</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/30066116</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/V6ruuTpiinDg6mgk9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/07/19/233-pantin-francia</t>
+  </si>
+  <si>
+    <t>Marguerites - Salvador Allende</t>
+  </si>
+  <si>
+    <t>Savigny-sur-Orge</t>
+  </si>
+  <si>
+    <t>91600</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/345141652</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/Uv9kXkNDfDMtDQ4X8</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/07/08/223-savigny-sur-orge-francia</t>
+  </si>
+  <si>
+    <t>Quartier Courbet</t>
+  </si>
+  <si>
+    <t>91390</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/379727574</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/ydJ5ZnzLkCGde96C9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/07/06/218-morsang-sur-orge-francia</t>
+  </si>
+  <si>
+    <t>Malakoff</t>
+  </si>
+  <si>
+    <t>92240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ville de Malakoff 
+Rue Salvador Allende 
+Président de la Répulique du Chili 
+Martyr de la liberté
+</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/24560374</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/G4CgbiEV3zUmKxXe8</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/07/02/217-malakoff-francia</t>
   </si>
 </sst>
 </file>
@@ -5936,8 +6363,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6264,14 +6693,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F527D2B3-F30A-4BB6-B445-B84E88C49493}">
-  <dimension ref="A1:Y353"/>
+  <dimension ref="A1:Y376"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A339" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B354" sqref="B354"/>
+      <pane ySplit="1" topLeftCell="A359" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B377" sqref="B377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="11" max="11" width="8.7265625" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -6378,7 +6810,7 @@
       <c r="J2" t="s">
         <v>33</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="3" t="s">
         <v>34</v>
       </c>
       <c r="L2">
@@ -6446,7 +6878,7 @@
       <c r="J3" t="s">
         <v>45</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="3" t="s">
         <v>46</v>
       </c>
       <c r="L3">
@@ -6505,7 +6937,7 @@
       <c r="J4" t="s">
         <v>54</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="3" t="s">
         <v>55</v>
       </c>
       <c r="L4">
@@ -6573,7 +7005,7 @@
       <c r="J5" t="s">
         <v>64</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="3" t="s">
         <v>65</v>
       </c>
       <c r="L5">
@@ -6635,7 +7067,7 @@
       <c r="J6" t="s">
         <v>71</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="3" t="s">
         <v>72</v>
       </c>
       <c r="L6">
@@ -6703,7 +7135,7 @@
       <c r="J7" t="s">
         <v>80</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="3" t="s">
         <v>81</v>
       </c>
       <c r="L7">
@@ -6768,7 +7200,7 @@
       <c r="J8" t="s">
         <v>89</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="3" t="s">
         <v>90</v>
       </c>
       <c r="L8">
@@ -6830,7 +7262,7 @@
       <c r="J9" t="s">
         <v>96</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="3" t="s">
         <v>97</v>
       </c>
       <c r="L9">
@@ -6889,7 +7321,7 @@
       <c r="J10" t="s">
         <v>103</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="3" t="s">
         <v>104</v>
       </c>
       <c r="L10">
@@ -6948,7 +7380,7 @@
       <c r="J11" t="s">
         <v>109</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="3" t="s">
         <v>110</v>
       </c>
       <c r="L11">
@@ -7016,7 +7448,7 @@
       <c r="J12" t="s">
         <v>117</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="3" t="s">
         <v>118</v>
       </c>
       <c r="L12">
@@ -7084,7 +7516,7 @@
       <c r="J13" t="s">
         <v>126</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="3" t="s">
         <v>127</v>
       </c>
       <c r="L13">
@@ -7143,7 +7575,7 @@
       <c r="J14" t="s">
         <v>133</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="3" t="s">
         <v>134</v>
       </c>
       <c r="L14">
@@ -7208,7 +7640,7 @@
       <c r="J15" t="s">
         <v>140</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="3" t="s">
         <v>141</v>
       </c>
       <c r="L15">
@@ -7270,7 +7702,7 @@
       <c r="J16" t="s">
         <v>146</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="3" t="s">
         <v>147</v>
       </c>
       <c r="L16">
@@ -7338,7 +7770,7 @@
       <c r="J17" t="s">
         <v>153</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="3" t="s">
         <v>154</v>
       </c>
       <c r="L17">
@@ -7400,7 +7832,7 @@
       <c r="J18" t="s">
         <v>159</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="3" t="s">
         <v>160</v>
       </c>
       <c r="L18">
@@ -7462,7 +7894,7 @@
       <c r="J19" t="s">
         <v>165</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="3" t="s">
         <v>166</v>
       </c>
       <c r="L19">
@@ -7524,7 +7956,7 @@
       <c r="J20" t="s">
         <v>171</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="3" t="s">
         <v>172</v>
       </c>
       <c r="L20">
@@ -7586,7 +8018,7 @@
       <c r="J21" t="s">
         <v>176</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="3" t="s">
         <v>177</v>
       </c>
       <c r="L21">
@@ -7645,7 +8077,7 @@
       <c r="I22" t="s">
         <v>181</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="3" t="s">
         <v>182</v>
       </c>
       <c r="L22">
@@ -7713,7 +8145,7 @@
       <c r="J23" t="s">
         <v>188</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="3" t="s">
         <v>189</v>
       </c>
       <c r="L23">
@@ -7772,7 +8204,7 @@
       <c r="J24" t="s">
         <v>194</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="3" t="s">
         <v>195</v>
       </c>
       <c r="L24">
@@ -7831,7 +8263,7 @@
       <c r="I25" t="s">
         <v>202</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="3" t="s">
         <v>203</v>
       </c>
       <c r="L25">
@@ -7893,7 +8325,7 @@
       <c r="J26" t="s">
         <v>208</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" s="3" t="s">
         <v>209</v>
       </c>
       <c r="L26">
@@ -7955,7 +8387,7 @@
       <c r="J27" t="s">
         <v>212</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="3" t="s">
         <v>213</v>
       </c>
       <c r="L27">
@@ -8017,7 +8449,7 @@
       <c r="J28" t="s">
         <v>217</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K28" s="3" t="s">
         <v>218</v>
       </c>
       <c r="L28">
@@ -8082,7 +8514,7 @@
       <c r="J29" t="s">
         <v>223</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K29" s="3" t="s">
         <v>224</v>
       </c>
       <c r="L29">
@@ -8144,7 +8576,7 @@
       <c r="J30" t="s">
         <v>229</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K30" s="3" t="s">
         <v>230</v>
       </c>
       <c r="L30">
@@ -8209,7 +8641,7 @@
       <c r="J31" t="s">
         <v>237</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="3" t="s">
         <v>238</v>
       </c>
       <c r="L31">
@@ -8268,7 +8700,7 @@
       <c r="J32" t="s">
         <v>243</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K32" s="3" t="s">
         <v>244</v>
       </c>
       <c r="L32">
@@ -8330,7 +8762,7 @@
       <c r="J33" t="s">
         <v>248</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K33" s="3" t="s">
         <v>249</v>
       </c>
       <c r="L33">
@@ -8395,7 +8827,7 @@
       <c r="J34" t="s">
         <v>253</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K34" s="3" t="s">
         <v>254</v>
       </c>
       <c r="L34">
@@ -8463,7 +8895,7 @@
       <c r="J35" t="s">
         <v>258</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K35" s="3" t="s">
         <v>259</v>
       </c>
       <c r="L35">
@@ -8525,7 +8957,7 @@
       <c r="J36" t="s">
         <v>262</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K36" s="3" t="s">
         <v>263</v>
       </c>
       <c r="L36">
@@ -8584,7 +9016,7 @@
       <c r="J37" t="s">
         <v>266</v>
       </c>
-      <c r="K37" t="s">
+      <c r="K37" s="3" t="s">
         <v>267</v>
       </c>
       <c r="L37">
@@ -8646,7 +9078,7 @@
       <c r="J38" t="s">
         <v>270</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K38" s="3" t="s">
         <v>271</v>
       </c>
       <c r="L38">
@@ -8708,7 +9140,7 @@
       <c r="J39" t="s">
         <v>276</v>
       </c>
-      <c r="K39" t="s">
+      <c r="K39" s="3" t="s">
         <v>277</v>
       </c>
       <c r="L39">
@@ -8770,7 +9202,7 @@
       <c r="J40" t="s">
         <v>281</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K40" s="3" t="s">
         <v>282</v>
       </c>
       <c r="L40">
@@ -8832,7 +9264,7 @@
       <c r="J41" t="s">
         <v>287</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K41" s="3" t="s">
         <v>288</v>
       </c>
       <c r="L41">
@@ -8897,7 +9329,7 @@
       <c r="J42" t="s">
         <v>294</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K42" s="3" t="s">
         <v>295</v>
       </c>
       <c r="L42">
@@ -8965,7 +9397,7 @@
       <c r="J43" t="s">
         <v>301</v>
       </c>
-      <c r="K43" t="s">
+      <c r="K43" s="3" t="s">
         <v>302</v>
       </c>
       <c r="L43">
@@ -9027,7 +9459,7 @@
       <c r="J44" t="s">
         <v>305</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K44" s="3" t="s">
         <v>306</v>
       </c>
       <c r="L44">
@@ -9086,7 +9518,7 @@
       <c r="J45" t="s">
         <v>311</v>
       </c>
-      <c r="K45" t="s">
+      <c r="K45" s="3" t="s">
         <v>312</v>
       </c>
       <c r="L45">
@@ -9145,7 +9577,7 @@
       <c r="I46" t="s">
         <v>316</v>
       </c>
-      <c r="K46" t="s">
+      <c r="K46" s="3" t="s">
         <v>317</v>
       </c>
       <c r="L46">
@@ -9201,7 +9633,7 @@
       <c r="I47" t="s">
         <v>321</v>
       </c>
-      <c r="K47" t="s">
+      <c r="K47" s="3" t="s">
         <v>322</v>
       </c>
       <c r="L47">
@@ -9260,7 +9692,7 @@
       <c r="J48" t="s">
         <v>326</v>
       </c>
-      <c r="K48" t="s">
+      <c r="K48" s="3" t="s">
         <v>327</v>
       </c>
       <c r="L48">
@@ -9322,7 +9754,7 @@
       <c r="J49" t="s">
         <v>333</v>
       </c>
-      <c r="K49" t="s">
+      <c r="K49" s="3" t="s">
         <v>334</v>
       </c>
       <c r="L49">
@@ -9381,7 +9813,7 @@
       <c r="J50" t="s">
         <v>337</v>
       </c>
-      <c r="K50" t="s">
+      <c r="K50" s="3" t="s">
         <v>338</v>
       </c>
       <c r="L50">
@@ -9449,7 +9881,7 @@
       <c r="J51" t="s">
         <v>345</v>
       </c>
-      <c r="K51" t="s">
+      <c r="K51" s="3" t="s">
         <v>346</v>
       </c>
       <c r="L51">
@@ -9517,7 +9949,7 @@
       <c r="J52" t="s">
         <v>351</v>
       </c>
-      <c r="K52" t="s">
+      <c r="K52" s="3" t="s">
         <v>352</v>
       </c>
       <c r="L52">
@@ -9576,7 +10008,7 @@
       <c r="J53" t="s">
         <v>358</v>
       </c>
-      <c r="K53" t="s">
+      <c r="K53" s="3" t="s">
         <v>359</v>
       </c>
       <c r="L53">
@@ -9638,7 +10070,7 @@
       <c r="J54" t="s">
         <v>365</v>
       </c>
-      <c r="K54" t="s">
+      <c r="K54" s="3" t="s">
         <v>366</v>
       </c>
       <c r="L54">
@@ -9697,7 +10129,7 @@
       <c r="I55" t="s">
         <v>370</v>
       </c>
-      <c r="K55" t="s">
+      <c r="K55" s="3" t="s">
         <v>371</v>
       </c>
       <c r="L55">
@@ -9824,7 +10256,7 @@
       <c r="I57" t="s">
         <v>383</v>
       </c>
-      <c r="K57" t="s">
+      <c r="K57" s="3" t="s">
         <v>384</v>
       </c>
       <c r="L57">
@@ -9892,7 +10324,7 @@
       <c r="J58" t="s">
         <v>389</v>
       </c>
-      <c r="K58" t="s">
+      <c r="K58" s="3" t="s">
         <v>390</v>
       </c>
       <c r="L58">
@@ -9951,7 +10383,7 @@
       <c r="J59" t="s">
         <v>394</v>
       </c>
-      <c r="K59" t="s">
+      <c r="K59" s="3" t="s">
         <v>395</v>
       </c>
       <c r="L59">
@@ -10016,7 +10448,7 @@
       <c r="J60" t="s">
         <v>399</v>
       </c>
-      <c r="K60" t="s">
+      <c r="K60" s="3" t="s">
         <v>400</v>
       </c>
       <c r="L60">
@@ -10078,7 +10510,7 @@
       <c r="J61" t="s">
         <v>405</v>
       </c>
-      <c r="K61" t="s">
+      <c r="K61" s="3" t="s">
         <v>406</v>
       </c>
       <c r="L61">
@@ -10140,7 +10572,7 @@
       <c r="J62" t="s">
         <v>410</v>
       </c>
-      <c r="K62" t="s">
+      <c r="K62" s="3" t="s">
         <v>411</v>
       </c>
       <c r="L62">
@@ -10202,7 +10634,7 @@
       <c r="J63" t="s">
         <v>416</v>
       </c>
-      <c r="K63" t="s">
+      <c r="K63" s="3" t="s">
         <v>417</v>
       </c>
       <c r="L63">
@@ -10261,7 +10693,7 @@
       <c r="J64" t="s">
         <v>421</v>
       </c>
-      <c r="K64" t="s">
+      <c r="K64" s="3" t="s">
         <v>422</v>
       </c>
       <c r="L64">
@@ -10323,7 +10755,7 @@
       <c r="J65" t="s">
         <v>427</v>
       </c>
-      <c r="K65" t="s">
+      <c r="K65" s="3" t="s">
         <v>428</v>
       </c>
       <c r="L65">
@@ -10382,7 +10814,7 @@
       <c r="J66" t="s">
         <v>433</v>
       </c>
-      <c r="K66" t="s">
+      <c r="K66" s="3" t="s">
         <v>434</v>
       </c>
       <c r="L66">
@@ -10441,7 +10873,7 @@
       <c r="I67" t="s">
         <v>439</v>
       </c>
-      <c r="K67" t="s">
+      <c r="K67" s="3" t="s">
         <v>440</v>
       </c>
       <c r="L67">
@@ -10503,7 +10935,7 @@
       <c r="J68" t="s">
         <v>444</v>
       </c>
-      <c r="K68" t="s">
+      <c r="K68" s="3" t="s">
         <v>445</v>
       </c>
       <c r="L68">
@@ -10624,7 +11056,7 @@
       <c r="I70" t="s">
         <v>88</v>
       </c>
-      <c r="K70" t="s">
+      <c r="K70" s="3" t="s">
         <v>456</v>
       </c>
       <c r="L70">
@@ -10686,7 +11118,7 @@
       <c r="J71" t="s">
         <v>461</v>
       </c>
-      <c r="K71" t="s">
+      <c r="K71" s="3" t="s">
         <v>462</v>
       </c>
       <c r="L71">
@@ -10748,7 +11180,7 @@
       <c r="J72" t="s">
         <v>465</v>
       </c>
-      <c r="K72" t="s">
+      <c r="K72" s="3" t="s">
         <v>466</v>
       </c>
       <c r="L72">
@@ -10810,7 +11242,7 @@
       <c r="J73" t="s">
         <v>471</v>
       </c>
-      <c r="K73" t="s">
+      <c r="K73" s="3" t="s">
         <v>472</v>
       </c>
       <c r="L73">
@@ -10925,7 +11357,7 @@
       <c r="I75" t="s">
         <v>481</v>
       </c>
-      <c r="K75" t="s">
+      <c r="K75" s="3" t="s">
         <v>482</v>
       </c>
       <c r="L75">
@@ -10987,7 +11419,7 @@
       <c r="J76" t="s">
         <v>487</v>
       </c>
-      <c r="K76" t="s">
+      <c r="K76" s="3" t="s">
         <v>488</v>
       </c>
       <c r="L76">
@@ -11049,7 +11481,7 @@
       <c r="J77" t="s">
         <v>493</v>
       </c>
-      <c r="K77" t="s">
+      <c r="K77" s="3" t="s">
         <v>494</v>
       </c>
       <c r="L77">
@@ -11114,7 +11546,7 @@
       <c r="I78" t="s">
         <v>499</v>
       </c>
-      <c r="K78" t="s">
+      <c r="K78" s="3" t="s">
         <v>500</v>
       </c>
       <c r="L78">
@@ -11182,7 +11614,7 @@
       <c r="J79" t="s">
         <v>506</v>
       </c>
-      <c r="K79" t="s">
+      <c r="K79" s="3" t="s">
         <v>507</v>
       </c>
       <c r="L79">
@@ -11244,7 +11676,7 @@
       <c r="J80" t="s">
         <v>511</v>
       </c>
-      <c r="K80" t="s">
+      <c r="K80" s="3" t="s">
         <v>238</v>
       </c>
       <c r="L80">
@@ -11303,7 +11735,7 @@
       <c r="J81" t="s">
         <v>516</v>
       </c>
-      <c r="K81" t="s">
+      <c r="K81" s="3" t="s">
         <v>517</v>
       </c>
       <c r="L81">
@@ -11365,7 +11797,7 @@
       <c r="J82" t="s">
         <v>520</v>
       </c>
-      <c r="K82" t="s">
+      <c r="K82" s="3" t="s">
         <v>521</v>
       </c>
       <c r="L82">
@@ -11430,7 +11862,7 @@
       <c r="J83" t="s">
         <v>526</v>
       </c>
-      <c r="K83" t="s">
+      <c r="K83" s="3" t="s">
         <v>527</v>
       </c>
       <c r="L83">
@@ -11492,7 +11924,7 @@
       <c r="J84" t="s">
         <v>533</v>
       </c>
-      <c r="K84" t="s">
+      <c r="K84" s="3" t="s">
         <v>534</v>
       </c>
       <c r="L84">
@@ -11551,7 +11983,7 @@
       <c r="J85" t="s">
         <v>539</v>
       </c>
-      <c r="K85" t="s">
+      <c r="K85" s="3" t="s">
         <v>540</v>
       </c>
       <c r="L85">
@@ -11610,7 +12042,7 @@
       <c r="J86" t="s">
         <v>545</v>
       </c>
-      <c r="K86" t="s">
+      <c r="K86" s="3" t="s">
         <v>546</v>
       </c>
       <c r="L86">
@@ -11675,7 +12107,7 @@
       <c r="J87" t="s">
         <v>551</v>
       </c>
-      <c r="K87" t="s">
+      <c r="K87" s="3" t="s">
         <v>552</v>
       </c>
       <c r="L87">
@@ -11743,7 +12175,7 @@
       <c r="J88" t="s">
         <v>559</v>
       </c>
-      <c r="K88" t="s">
+      <c r="K88" s="3" t="s">
         <v>560</v>
       </c>
       <c r="L88">
@@ -11805,7 +12237,7 @@
       <c r="J89" t="s">
         <v>564</v>
       </c>
-      <c r="K89" t="s">
+      <c r="K89" s="3" t="s">
         <v>565</v>
       </c>
       <c r="L89">
@@ -11867,7 +12299,7 @@
       <c r="J90" t="s">
         <v>568</v>
       </c>
-      <c r="K90" t="s">
+      <c r="K90" s="3" t="s">
         <v>569</v>
       </c>
       <c r="L90">
@@ -11926,7 +12358,7 @@
       <c r="J91" t="s">
         <v>574</v>
       </c>
-      <c r="K91" t="s">
+      <c r="K91" s="3" t="s">
         <v>575</v>
       </c>
       <c r="L91">
@@ -11988,7 +12420,7 @@
       <c r="J92" t="s">
         <v>579</v>
       </c>
-      <c r="K92" t="s">
+      <c r="K92" s="3" t="s">
         <v>580</v>
       </c>
       <c r="L92">
@@ -12047,7 +12479,7 @@
       <c r="J93" t="s">
         <v>584</v>
       </c>
-      <c r="K93" t="s">
+      <c r="K93" s="3" t="s">
         <v>585</v>
       </c>
       <c r="L93">
@@ -12106,7 +12538,7 @@
       <c r="J94" t="s">
         <v>589</v>
       </c>
-      <c r="K94" t="s">
+      <c r="K94" s="3" t="s">
         <v>590</v>
       </c>
       <c r="L94">
@@ -12165,7 +12597,7 @@
       <c r="J95" t="s">
         <v>595</v>
       </c>
-      <c r="K95" t="s">
+      <c r="K95" s="3" t="s">
         <v>596</v>
       </c>
       <c r="L95">
@@ -12317,7 +12749,7 @@
         <v>662</v>
       </c>
       <c r="Y97" s="2" t="s">
-        <v>599</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="98" spans="2:25" x14ac:dyDescent="0.35">
@@ -12376,7 +12808,7 @@
         <v>608</v>
       </c>
       <c r="Y98" s="2" t="s">
-        <v>599</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="99" spans="2:25" x14ac:dyDescent="0.35">
@@ -12466,7 +12898,7 @@
       <c r="J100" t="s">
         <v>615</v>
       </c>
-      <c r="K100" t="s">
+      <c r="K100" s="3" t="s">
         <v>616</v>
       </c>
       <c r="L100">
@@ -12525,7 +12957,7 @@
       <c r="J101" t="s">
         <v>622</v>
       </c>
-      <c r="K101" t="s">
+      <c r="K101" s="3" t="s">
         <v>623</v>
       </c>
       <c r="L101">
@@ -12587,7 +13019,7 @@
       <c r="J102" t="s">
         <v>627</v>
       </c>
-      <c r="K102" t="s">
+      <c r="K102" s="3" t="s">
         <v>628</v>
       </c>
       <c r="L102">
@@ -12646,7 +13078,7 @@
       <c r="I103" t="s">
         <v>633</v>
       </c>
-      <c r="K103" t="s">
+      <c r="K103" s="3" t="s">
         <v>634</v>
       </c>
       <c r="L103">
@@ -12708,7 +13140,7 @@
       <c r="J104" t="s">
         <v>640</v>
       </c>
-      <c r="K104" t="s">
+      <c r="K104" s="3" t="s">
         <v>641</v>
       </c>
       <c r="L104">
@@ -12770,7 +13202,7 @@
       <c r="J105" t="s">
         <v>647</v>
       </c>
-      <c r="K105" t="s">
+      <c r="K105" s="3" t="s">
         <v>648</v>
       </c>
       <c r="L105">
@@ -12829,7 +13261,7 @@
       <c r="J106" t="s">
         <v>652</v>
       </c>
-      <c r="K106" t="s">
+      <c r="K106" s="3" t="s">
         <v>653</v>
       </c>
       <c r="L106">
@@ -12891,7 +13323,7 @@
       <c r="J107" t="s">
         <v>658</v>
       </c>
-      <c r="K107" t="s">
+      <c r="K107" s="3" t="s">
         <v>659</v>
       </c>
       <c r="L107">
@@ -12953,7 +13385,7 @@
       <c r="J108" t="s">
         <v>665</v>
       </c>
-      <c r="K108" t="s">
+      <c r="K108" s="3" t="s">
         <v>666</v>
       </c>
       <c r="L108">
@@ -13015,7 +13447,7 @@
       <c r="J109" t="s">
         <v>665</v>
       </c>
-      <c r="K109" t="s">
+      <c r="K109" s="3" t="s">
         <v>666</v>
       </c>
       <c r="L109">
@@ -13077,7 +13509,7 @@
       <c r="J110" t="s">
         <v>674</v>
       </c>
-      <c r="K110" t="s">
+      <c r="K110" s="3" t="s">
         <v>675</v>
       </c>
       <c r="L110">
@@ -13139,7 +13571,7 @@
       <c r="J111" t="s">
         <v>680</v>
       </c>
-      <c r="K111" t="s">
+      <c r="K111" s="3" t="s">
         <v>681</v>
       </c>
       <c r="L111">
@@ -13207,7 +13639,7 @@
       <c r="J112" t="s">
         <v>685</v>
       </c>
-      <c r="K112" t="s">
+      <c r="K112" s="3" t="s">
         <v>686</v>
       </c>
       <c r="L112">
@@ -13269,7 +13701,7 @@
       <c r="J113" t="s">
         <v>690</v>
       </c>
-      <c r="K113" t="s">
+      <c r="K113" s="3" t="s">
         <v>691</v>
       </c>
       <c r="L113">
@@ -13334,7 +13766,7 @@
       <c r="J114" t="s">
         <v>695</v>
       </c>
-      <c r="K114" t="s">
+      <c r="K114" s="3" t="s">
         <v>696</v>
       </c>
       <c r="L114">
@@ -13402,7 +13834,7 @@
       <c r="J115" t="s">
         <v>702</v>
       </c>
-      <c r="K115" t="s">
+      <c r="K115" s="3" t="s">
         <v>703</v>
       </c>
       <c r="L115">
@@ -13461,7 +13893,7 @@
       <c r="I116" t="s">
         <v>710</v>
       </c>
-      <c r="K116" t="s">
+      <c r="K116" s="3" t="s">
         <v>711</v>
       </c>
       <c r="L116">
@@ -13523,7 +13955,7 @@
       <c r="J117" t="s">
         <v>714</v>
       </c>
-      <c r="K117" t="s">
+      <c r="K117" s="3" t="s">
         <v>715</v>
       </c>
       <c r="L117">
@@ -13585,7 +14017,7 @@
       <c r="J118" t="s">
         <v>721</v>
       </c>
-      <c r="K118" t="s">
+      <c r="K118" s="3" t="s">
         <v>722</v>
       </c>
       <c r="L118">
@@ -13644,7 +14076,7 @@
       <c r="J119" t="s">
         <v>727</v>
       </c>
-      <c r="K119" t="s">
+      <c r="K119" s="3" t="s">
         <v>728</v>
       </c>
       <c r="L119">
@@ -13712,7 +14144,7 @@
       <c r="J120" t="s">
         <v>736</v>
       </c>
-      <c r="K120" t="s">
+      <c r="K120" s="3" t="s">
         <v>737</v>
       </c>
       <c r="L120">
@@ -13774,7 +14206,7 @@
       <c r="J121" t="s">
         <v>743</v>
       </c>
-      <c r="K121" t="s">
+      <c r="K121" s="3" t="s">
         <v>744</v>
       </c>
       <c r="L121">
@@ -13830,7 +14262,7 @@
       <c r="J122" t="s">
         <v>747</v>
       </c>
-      <c r="K122" t="s">
+      <c r="K122" s="3" t="s">
         <v>748</v>
       </c>
       <c r="L122">
@@ -13892,7 +14324,7 @@
       <c r="J123" t="s">
         <v>752</v>
       </c>
-      <c r="K123" t="s">
+      <c r="K123" s="3" t="s">
         <v>753</v>
       </c>
       <c r="L123">
@@ -13954,7 +14386,7 @@
       <c r="J124" t="s">
         <v>757</v>
       </c>
-      <c r="K124" t="s">
+      <c r="K124" s="3" t="s">
         <v>758</v>
       </c>
       <c r="L124">
@@ -14016,7 +14448,7 @@
       <c r="J125" t="s">
         <v>761</v>
       </c>
-      <c r="K125" t="s">
+      <c r="K125" s="3" t="s">
         <v>762</v>
       </c>
       <c r="L125">
@@ -14075,7 +14507,7 @@
       <c r="J126" t="s">
         <v>766</v>
       </c>
-      <c r="K126" t="s">
+      <c r="K126" s="3" t="s">
         <v>767</v>
       </c>
       <c r="L126">
@@ -14137,7 +14569,7 @@
       <c r="J127" t="s">
         <v>770</v>
       </c>
-      <c r="K127" t="s">
+      <c r="K127" s="3" t="s">
         <v>771</v>
       </c>
       <c r="L127">
@@ -14196,7 +14628,7 @@
       <c r="J128" t="s">
         <v>774</v>
       </c>
-      <c r="K128" t="s">
+      <c r="K128" s="3" t="s">
         <v>775</v>
       </c>
       <c r="L128">
@@ -14258,7 +14690,7 @@
       <c r="J129" t="s">
         <v>780</v>
       </c>
-      <c r="K129" t="s">
+      <c r="K129" s="3" t="s">
         <v>781</v>
       </c>
       <c r="L129">
@@ -14317,7 +14749,7 @@
       <c r="J130" t="s">
         <v>784</v>
       </c>
-      <c r="K130" t="s">
+      <c r="K130" s="3" t="s">
         <v>785</v>
       </c>
       <c r="L130">
@@ -14379,7 +14811,7 @@
       <c r="J131" t="s">
         <v>788</v>
       </c>
-      <c r="K131" t="s">
+      <c r="K131" s="3" t="s">
         <v>789</v>
       </c>
       <c r="L131">
@@ -14447,7 +14879,7 @@
       <c r="J132" t="s">
         <v>795</v>
       </c>
-      <c r="K132" t="s">
+      <c r="K132" s="3" t="s">
         <v>796</v>
       </c>
       <c r="L132">
@@ -14512,7 +14944,7 @@
       <c r="J133" t="s">
         <v>801</v>
       </c>
-      <c r="K133" t="s">
+      <c r="K133" s="3" t="s">
         <v>802</v>
       </c>
       <c r="L133">
@@ -14580,7 +15012,7 @@
       <c r="J134" t="s">
         <v>806</v>
       </c>
-      <c r="K134" t="s">
+      <c r="K134" s="3" t="s">
         <v>807</v>
       </c>
       <c r="L134">
@@ -14648,7 +15080,7 @@
       <c r="J135" t="s">
         <v>812</v>
       </c>
-      <c r="K135" t="s">
+      <c r="K135" s="3" t="s">
         <v>813</v>
       </c>
       <c r="L135">
@@ -14710,7 +15142,7 @@
       <c r="J136" t="s">
         <v>817</v>
       </c>
-      <c r="K136" t="s">
+      <c r="K136" s="3" t="s">
         <v>818</v>
       </c>
       <c r="L136">
@@ -14834,7 +15266,7 @@
       <c r="J138" t="s">
         <v>827</v>
       </c>
-      <c r="K138" t="s">
+      <c r="K138" s="3" t="s">
         <v>828</v>
       </c>
       <c r="L138">
@@ -14896,7 +15328,7 @@
       <c r="J139" t="s">
         <v>834</v>
       </c>
-      <c r="K139" t="s">
+      <c r="K139" s="3" t="s">
         <v>835</v>
       </c>
       <c r="L139">
@@ -14955,7 +15387,7 @@
       <c r="J140" t="s">
         <v>838</v>
       </c>
-      <c r="K140" t="s">
+      <c r="K140" s="3" t="s">
         <v>839</v>
       </c>
       <c r="L140">
@@ -15017,7 +15449,7 @@
       <c r="J141" t="s">
         <v>843</v>
       </c>
-      <c r="K141" t="s">
+      <c r="K141" s="3" t="s">
         <v>844</v>
       </c>
       <c r="L141">
@@ -15079,7 +15511,7 @@
       <c r="J142" t="s">
         <v>849</v>
       </c>
-      <c r="K142" t="s">
+      <c r="K142" s="3" t="s">
         <v>850</v>
       </c>
       <c r="L142">
@@ -15138,7 +15570,7 @@
       <c r="J143" t="s">
         <v>853</v>
       </c>
-      <c r="K143" t="s">
+      <c r="K143" s="3" t="s">
         <v>854</v>
       </c>
       <c r="L143">
@@ -15197,7 +15629,7 @@
       <c r="J144" t="s">
         <v>857</v>
       </c>
-      <c r="K144" t="s">
+      <c r="K144" s="3" t="s">
         <v>858</v>
       </c>
       <c r="L144">
@@ -15256,7 +15688,7 @@
       <c r="J145" t="s">
         <v>863</v>
       </c>
-      <c r="K145" t="s">
+      <c r="K145" s="3" t="s">
         <v>864</v>
       </c>
       <c r="L145">
@@ -15318,7 +15750,7 @@
       <c r="J146" t="s">
         <v>448</v>
       </c>
-      <c r="K146" t="s">
+      <c r="K146" s="3" t="s">
         <v>867</v>
       </c>
       <c r="L146">
@@ -15377,7 +15809,7 @@
       <c r="J147" t="s">
         <v>870</v>
       </c>
-      <c r="K147" t="s">
+      <c r="K147" s="3" t="s">
         <v>871</v>
       </c>
       <c r="L147">
@@ -15439,7 +15871,7 @@
       <c r="J148" t="s">
         <v>875</v>
       </c>
-      <c r="K148" t="s">
+      <c r="K148" s="3" t="s">
         <v>876</v>
       </c>
       <c r="L148">
@@ -15501,7 +15933,7 @@
       <c r="J149" t="s">
         <v>882</v>
       </c>
-      <c r="K149" t="s">
+      <c r="K149" s="3" t="s">
         <v>883</v>
       </c>
       <c r="L149">
@@ -15563,7 +15995,7 @@
       <c r="J150" t="s">
         <v>886</v>
       </c>
-      <c r="K150" t="s">
+      <c r="K150" s="3" t="s">
         <v>887</v>
       </c>
       <c r="L150">
@@ -15622,7 +16054,7 @@
       <c r="J151" t="s">
         <v>891</v>
       </c>
-      <c r="K151" t="s">
+      <c r="K151" s="3" t="s">
         <v>892</v>
       </c>
       <c r="L151">
@@ -15684,7 +16116,7 @@
       <c r="J152" t="s">
         <v>896</v>
       </c>
-      <c r="K152" t="s">
+      <c r="K152" s="3" t="s">
         <v>897</v>
       </c>
       <c r="L152">
@@ -15746,7 +16178,7 @@
       <c r="J153" t="s">
         <v>902</v>
       </c>
-      <c r="K153" t="s">
+      <c r="K153" s="3" t="s">
         <v>903</v>
       </c>
       <c r="L153">
@@ -15808,7 +16240,7 @@
       <c r="J154" t="s">
         <v>907</v>
       </c>
-      <c r="K154" t="s">
+      <c r="K154" s="3" t="s">
         <v>908</v>
       </c>
       <c r="L154">
@@ -15870,7 +16302,7 @@
       <c r="J155" t="s">
         <v>913</v>
       </c>
-      <c r="K155" t="s">
+      <c r="K155" s="3" t="s">
         <v>914</v>
       </c>
       <c r="L155">
@@ -15932,7 +16364,7 @@
       <c r="J156" t="s">
         <v>917</v>
       </c>
-      <c r="K156" t="s">
+      <c r="K156" s="3" t="s">
         <v>918</v>
       </c>
       <c r="L156">
@@ -15994,7 +16426,7 @@
       <c r="J157" t="s">
         <v>921</v>
       </c>
-      <c r="K157" t="s">
+      <c r="K157" s="3" t="s">
         <v>922</v>
       </c>
       <c r="L157">
@@ -16053,7 +16485,7 @@
       <c r="J158" t="s">
         <v>926</v>
       </c>
-      <c r="K158" t="s">
+      <c r="K158" s="3" t="s">
         <v>927</v>
       </c>
       <c r="L158">
@@ -16115,7 +16547,7 @@
       <c r="J159" t="s">
         <v>931</v>
       </c>
-      <c r="K159" t="s">
+      <c r="K159" s="3" t="s">
         <v>932</v>
       </c>
       <c r="L159">
@@ -16177,7 +16609,7 @@
       <c r="J160" t="s">
         <v>935</v>
       </c>
-      <c r="K160" t="s">
+      <c r="K160" s="3" t="s">
         <v>936</v>
       </c>
       <c r="L160">
@@ -16239,7 +16671,7 @@
       <c r="J161" t="s">
         <v>939</v>
       </c>
-      <c r="K161" t="s">
+      <c r="K161" s="3" t="s">
         <v>940</v>
       </c>
       <c r="L161">
@@ -16301,7 +16733,7 @@
       <c r="J162" t="s">
         <v>380</v>
       </c>
-      <c r="K162" t="s">
+      <c r="K162" s="3" t="s">
         <v>943</v>
       </c>
       <c r="L162">
@@ -16360,7 +16792,7 @@
       <c r="J163" t="s">
         <v>946</v>
       </c>
-      <c r="K163" t="s">
+      <c r="K163" s="3" t="s">
         <v>947</v>
       </c>
       <c r="L163">
@@ -16425,7 +16857,7 @@
       <c r="I164" t="s">
         <v>953</v>
       </c>
-      <c r="K164" t="s">
+      <c r="K164" s="3" t="s">
         <v>954</v>
       </c>
       <c r="L164">
@@ -16487,7 +16919,7 @@
       <c r="J165" t="s">
         <v>958</v>
       </c>
-      <c r="K165" t="s">
+      <c r="K165" s="3" t="s">
         <v>959</v>
       </c>
       <c r="L165">
@@ -16549,7 +16981,7 @@
       <c r="J166" t="s">
         <v>962</v>
       </c>
-      <c r="K166" t="s">
+      <c r="K166" s="3" t="s">
         <v>963</v>
       </c>
       <c r="L166">
@@ -16611,7 +17043,7 @@
       <c r="J167" t="s">
         <v>966</v>
       </c>
-      <c r="K167" t="s">
+      <c r="K167" s="3" t="s">
         <v>967</v>
       </c>
       <c r="L167">
@@ -16670,7 +17102,7 @@
       <c r="J168" t="s">
         <v>972</v>
       </c>
-      <c r="K168" t="s">
+      <c r="K168" s="3" t="s">
         <v>973</v>
       </c>
       <c r="L168">
@@ -16729,7 +17161,7 @@
       <c r="J169" t="s">
         <v>976</v>
       </c>
-      <c r="K169" t="s">
+      <c r="K169" s="3" t="s">
         <v>977</v>
       </c>
       <c r="L169">
@@ -16791,7 +17223,7 @@
       <c r="J170" t="s">
         <v>981</v>
       </c>
-      <c r="K170" t="s">
+      <c r="K170" s="3" t="s">
         <v>982</v>
       </c>
       <c r="L170">
@@ -16850,7 +17282,7 @@
       <c r="J171" t="s">
         <v>985</v>
       </c>
-      <c r="K171" t="s">
+      <c r="K171" s="3" t="s">
         <v>986</v>
       </c>
       <c r="L171">
@@ -16909,7 +17341,7 @@
       <c r="J172" t="s">
         <v>990</v>
       </c>
-      <c r="K172" t="s">
+      <c r="K172" s="3" t="s">
         <v>991</v>
       </c>
       <c r="L172">
@@ -16968,7 +17400,7 @@
       <c r="J173" t="s">
         <v>994</v>
       </c>
-      <c r="K173" t="s">
+      <c r="K173" s="3" t="s">
         <v>995</v>
       </c>
       <c r="L173">
@@ -17033,7 +17465,7 @@
       <c r="J174" t="s">
         <v>1000</v>
       </c>
-      <c r="K174" t="s">
+      <c r="K174" s="3" t="s">
         <v>1001</v>
       </c>
       <c r="L174">
@@ -17101,7 +17533,7 @@
       <c r="J175" t="s">
         <v>1005</v>
       </c>
-      <c r="K175" t="s">
+      <c r="K175" s="3" t="s">
         <v>1006</v>
       </c>
       <c r="L175">
@@ -17166,7 +17598,7 @@
       <c r="J176" t="s">
         <v>1010</v>
       </c>
-      <c r="K176" t="s">
+      <c r="K176" s="3" t="s">
         <v>1011</v>
       </c>
       <c r="L176">
@@ -17225,7 +17657,7 @@
       <c r="J177" t="s">
         <v>1016</v>
       </c>
-      <c r="K177" t="s">
+      <c r="K177" s="3" t="s">
         <v>1017</v>
       </c>
       <c r="L177">
@@ -17287,7 +17719,7 @@
       <c r="J178" t="s">
         <v>1023</v>
       </c>
-      <c r="K178" t="s">
+      <c r="K178" s="3" t="s">
         <v>1024</v>
       </c>
       <c r="L178">
@@ -17349,7 +17781,7 @@
       <c r="J179" t="s">
         <v>1028</v>
       </c>
-      <c r="K179" t="s">
+      <c r="K179" s="3" t="s">
         <v>1029</v>
       </c>
       <c r="L179">
@@ -17408,7 +17840,7 @@
       <c r="I180" t="s">
         <v>1032</v>
       </c>
-      <c r="K180" t="s">
+      <c r="K180" s="3" t="s">
         <v>1033</v>
       </c>
       <c r="L180">
@@ -17470,7 +17902,7 @@
       <c r="J181" t="s">
         <v>1170</v>
       </c>
-      <c r="K181" s="4" t="s">
+      <c r="K181" s="5" t="s">
         <v>1033</v>
       </c>
       <c r="L181">
@@ -17533,7 +17965,7 @@
       <c r="J182" t="s">
         <v>1037</v>
       </c>
-      <c r="K182" t="s">
+      <c r="K182" s="3" t="s">
         <v>1038</v>
       </c>
       <c r="L182">
@@ -17595,7 +18027,7 @@
       <c r="J183" t="s">
         <v>1041</v>
       </c>
-      <c r="K183" t="s">
+      <c r="K183" s="3" t="s">
         <v>1042</v>
       </c>
       <c r="L183">
@@ -17657,7 +18089,7 @@
       <c r="J184" t="s">
         <v>1046</v>
       </c>
-      <c r="K184" t="s">
+      <c r="K184" s="3" t="s">
         <v>1047</v>
       </c>
       <c r="L184">
@@ -17725,7 +18157,7 @@
       <c r="J185" t="s">
         <v>1052</v>
       </c>
-      <c r="K185" t="s">
+      <c r="K185" s="3" t="s">
         <v>1053</v>
       </c>
       <c r="L185">
@@ -17787,7 +18219,7 @@
       <c r="J186" t="s">
         <v>1056</v>
       </c>
-      <c r="K186" t="s">
+      <c r="K186" s="3" t="s">
         <v>1057</v>
       </c>
       <c r="L186">
@@ -17849,7 +18281,7 @@
       <c r="J187" t="s">
         <v>1061</v>
       </c>
-      <c r="K187" t="s">
+      <c r="K187" s="3" t="s">
         <v>1062</v>
       </c>
       <c r="L187">
@@ -17911,7 +18343,7 @@
       <c r="J188" t="s">
         <v>1067</v>
       </c>
-      <c r="K188" t="s">
+      <c r="K188" s="3" t="s">
         <v>1068</v>
       </c>
       <c r="L188">
@@ -17970,7 +18402,7 @@
       <c r="J189" t="s">
         <v>1072</v>
       </c>
-      <c r="K189" t="s">
+      <c r="K189" s="3" t="s">
         <v>1073</v>
       </c>
       <c r="L189">
@@ -18038,7 +18470,7 @@
       <c r="J190" t="s">
         <v>1077</v>
       </c>
-      <c r="K190" t="s">
+      <c r="K190" s="3" t="s">
         <v>1078</v>
       </c>
       <c r="L190">
@@ -18097,7 +18529,7 @@
       <c r="J191" t="s">
         <v>1081</v>
       </c>
-      <c r="K191" t="s">
+      <c r="K191" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="L191">
@@ -18156,7 +18588,7 @@
       <c r="J192" t="s">
         <v>1086</v>
       </c>
-      <c r="K192" t="s">
+      <c r="K192" s="3" t="s">
         <v>1087</v>
       </c>
       <c r="L192">
@@ -18212,7 +18644,7 @@
       <c r="I193" t="s">
         <v>1091</v>
       </c>
-      <c r="K193" t="s">
+      <c r="K193" s="3" t="s">
         <v>1092</v>
       </c>
       <c r="L193">
@@ -18280,7 +18712,7 @@
       <c r="J194" t="s">
         <v>1097</v>
       </c>
-      <c r="K194" t="s">
+      <c r="K194" s="3" t="s">
         <v>1098</v>
       </c>
       <c r="L194">
@@ -18348,7 +18780,7 @@
       <c r="J195" t="s">
         <v>1102</v>
       </c>
-      <c r="K195" t="s">
+      <c r="K195" s="3" t="s">
         <v>1103</v>
       </c>
       <c r="L195">
@@ -18410,7 +18842,7 @@
       <c r="J196" t="s">
         <v>1106</v>
       </c>
-      <c r="K196" t="s">
+      <c r="K196" s="3" t="s">
         <v>1107</v>
       </c>
       <c r="L196">
@@ -18466,7 +18898,7 @@
       <c r="I197" t="s">
         <v>1111</v>
       </c>
-      <c r="K197" t="s">
+      <c r="K197" s="3" t="s">
         <v>1112</v>
       </c>
       <c r="L197">
@@ -18525,7 +18957,7 @@
       <c r="I198" t="s">
         <v>1115</v>
       </c>
-      <c r="K198" t="s">
+      <c r="K198" s="3" t="s">
         <v>1116</v>
       </c>
       <c r="L198">
@@ -18593,7 +19025,7 @@
       <c r="J199" t="s">
         <v>1120</v>
       </c>
-      <c r="K199" t="s">
+      <c r="K199" s="3" t="s">
         <v>1121</v>
       </c>
       <c r="L199">
@@ -18652,7 +19084,7 @@
       <c r="J200" t="s">
         <v>1126</v>
       </c>
-      <c r="K200" t="s">
+      <c r="K200" s="3" t="s">
         <v>1127</v>
       </c>
       <c r="L200">
@@ -18714,7 +19146,7 @@
       <c r="J201" t="s">
         <v>1131</v>
       </c>
-      <c r="K201" t="s">
+      <c r="K201" s="3" t="s">
         <v>1132</v>
       </c>
       <c r="L201">
@@ -18773,7 +19205,7 @@
       <c r="I202" t="s">
         <v>1136</v>
       </c>
-      <c r="K202" t="s">
+      <c r="K202" s="3" t="s">
         <v>1137</v>
       </c>
       <c r="L202">
@@ -18835,7 +19267,7 @@
       <c r="J203" t="s">
         <v>1140</v>
       </c>
-      <c r="K203" t="s">
+      <c r="K203" s="3" t="s">
         <v>1141</v>
       </c>
       <c r="L203">
@@ -18894,7 +19326,7 @@
       <c r="I204" t="s">
         <v>1144</v>
       </c>
-      <c r="K204" t="s">
+      <c r="K204" s="3" t="s">
         <v>1145</v>
       </c>
       <c r="L204">
@@ -18956,7 +19388,7 @@
       <c r="J205" t="s">
         <v>1148</v>
       </c>
-      <c r="K205" t="s">
+      <c r="K205" s="3" t="s">
         <v>653</v>
       </c>
       <c r="L205">
@@ -19018,7 +19450,7 @@
       <c r="J206" t="s">
         <v>1151</v>
       </c>
-      <c r="K206" t="s">
+      <c r="K206" s="3" t="s">
         <v>1152</v>
       </c>
       <c r="L206">
@@ -19074,7 +19506,7 @@
       <c r="I207" t="s">
         <v>1156</v>
       </c>
-      <c r="K207" t="s">
+      <c r="K207" s="3" t="s">
         <v>1157</v>
       </c>
       <c r="L207">
@@ -19136,7 +19568,7 @@
       <c r="J208" t="s">
         <v>1161</v>
       </c>
-      <c r="K208" t="s">
+      <c r="K208" s="3" t="s">
         <v>1162</v>
       </c>
       <c r="L208">
@@ -19204,7 +19636,7 @@
       <c r="J209" t="s">
         <v>1166</v>
       </c>
-      <c r="K209" t="s">
+      <c r="K209" s="3" t="s">
         <v>1167</v>
       </c>
       <c r="L209">
@@ -19266,7 +19698,7 @@
       <c r="J210" t="s">
         <v>1176</v>
       </c>
-      <c r="K210" s="4" t="s">
+      <c r="K210" s="5" t="s">
         <v>1177</v>
       </c>
       <c r="L210">
@@ -19287,10 +19719,10 @@
       <c r="V210">
         <v>1</v>
       </c>
-      <c r="W210" s="5" t="s">
+      <c r="W210" s="4" t="s">
         <v>1174</v>
       </c>
-      <c r="X210" s="5" t="s">
+      <c r="X210" s="4" t="s">
         <v>1178</v>
       </c>
     </row>
@@ -19322,7 +19754,7 @@
       <c r="J211" t="s">
         <v>1181</v>
       </c>
-      <c r="K211" t="s">
+      <c r="K211" s="3" t="s">
         <v>1182</v>
       </c>
       <c r="L211">
@@ -19384,7 +19816,7 @@
       <c r="J212" t="s">
         <v>1188</v>
       </c>
-      <c r="K212" t="s">
+      <c r="K212" s="3" t="s">
         <v>1189</v>
       </c>
       <c r="L212">
@@ -19446,7 +19878,7 @@
       <c r="J213" t="s">
         <v>1193</v>
       </c>
-      <c r="K213" t="s">
+      <c r="K213" s="3" t="s">
         <v>1194</v>
       </c>
       <c r="L213">
@@ -19502,7 +19934,7 @@
       <c r="I214" t="s">
         <v>1198</v>
       </c>
-      <c r="K214" t="s">
+      <c r="K214" s="3" t="s">
         <v>1199</v>
       </c>
       <c r="L214">
@@ -19564,7 +19996,7 @@
       <c r="J215" t="s">
         <v>1202</v>
       </c>
-      <c r="K215" t="s">
+      <c r="K215" s="3" t="s">
         <v>1203</v>
       </c>
       <c r="L215">
@@ -19623,7 +20055,7 @@
       <c r="J216" t="s">
         <v>1206</v>
       </c>
-      <c r="K216" t="s">
+      <c r="K216" s="3" t="s">
         <v>1207</v>
       </c>
       <c r="L216">
@@ -19682,7 +20114,7 @@
       <c r="J217" t="s">
         <v>1210</v>
       </c>
-      <c r="K217" t="s">
+      <c r="K217" s="3" t="s">
         <v>1211</v>
       </c>
       <c r="L217">
@@ -19741,7 +20173,7 @@
       <c r="J218" t="s">
         <v>1215</v>
       </c>
-      <c r="K218" t="s">
+      <c r="K218" s="3" t="s">
         <v>1216</v>
       </c>
       <c r="L218">
@@ -19800,7 +20232,7 @@
       <c r="J219" t="s">
         <v>1219</v>
       </c>
-      <c r="K219" t="s">
+      <c r="K219" s="3" t="s">
         <v>1220</v>
       </c>
       <c r="L219">
@@ -19862,7 +20294,7 @@
       <c r="J220" t="s">
         <v>1223</v>
       </c>
-      <c r="K220" t="s">
+      <c r="K220" s="3" t="s">
         <v>1224</v>
       </c>
       <c r="L220">
@@ -19921,7 +20353,7 @@
       <c r="J221" t="s">
         <v>1227</v>
       </c>
-      <c r="K221" t="s">
+      <c r="K221" s="3" t="s">
         <v>1228</v>
       </c>
       <c r="L221">
@@ -19980,7 +20412,7 @@
       <c r="J222" t="s">
         <v>1232</v>
       </c>
-      <c r="K222" t="s">
+      <c r="K222" s="3" t="s">
         <v>1233</v>
       </c>
       <c r="L222">
@@ -20039,7 +20471,7 @@
       <c r="J223" t="s">
         <v>1236</v>
       </c>
-      <c r="K223" t="s">
+      <c r="K223" s="3" t="s">
         <v>1237</v>
       </c>
       <c r="L223">
@@ -20095,7 +20527,7 @@
       <c r="I224" t="s">
         <v>1240</v>
       </c>
-      <c r="K224" t="s">
+      <c r="K224" s="3" t="s">
         <v>1241</v>
       </c>
       <c r="L224">
@@ -20157,7 +20589,7 @@
       <c r="J225" t="s">
         <v>1245</v>
       </c>
-      <c r="K225" t="s">
+      <c r="K225" s="3" t="s">
         <v>1246</v>
       </c>
       <c r="L225">
@@ -20219,7 +20651,7 @@
       <c r="J226" t="s">
         <v>1250</v>
       </c>
-      <c r="K226" t="s">
+      <c r="K226" s="3" t="s">
         <v>1251</v>
       </c>
       <c r="L226">
@@ -20278,7 +20710,7 @@
       <c r="J227" t="s">
         <v>1254</v>
       </c>
-      <c r="K227" t="s">
+      <c r="K227" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="L227">
@@ -20337,7 +20769,7 @@
       <c r="I228" t="s">
         <v>1258</v>
       </c>
-      <c r="K228" t="s">
+      <c r="K228" s="3" t="s">
         <v>1259</v>
       </c>
       <c r="L228">
@@ -20399,7 +20831,7 @@
       <c r="J229" t="s">
         <v>1264</v>
       </c>
-      <c r="K229" t="s">
+      <c r="K229" s="3" t="s">
         <v>1265</v>
       </c>
       <c r="L229">
@@ -20461,7 +20893,7 @@
       <c r="J230" t="s">
         <v>1268</v>
       </c>
-      <c r="K230" t="s">
+      <c r="K230" s="3" t="s">
         <v>1269</v>
       </c>
       <c r="L230">
@@ -20520,7 +20952,7 @@
       <c r="J231" t="s">
         <v>1273</v>
       </c>
-      <c r="K231" t="s">
+      <c r="K231" s="3" t="s">
         <v>1274</v>
       </c>
       <c r="L231">
@@ -20579,7 +21011,7 @@
       <c r="J232" t="s">
         <v>1277</v>
       </c>
-      <c r="K232" t="s">
+      <c r="K232" s="3" t="s">
         <v>1278</v>
       </c>
       <c r="L232">
@@ -20638,7 +21070,7 @@
       <c r="J233" t="s">
         <v>1281</v>
       </c>
-      <c r="K233" t="s">
+      <c r="K233" s="3" t="s">
         <v>1282</v>
       </c>
       <c r="L233">
@@ -20697,7 +21129,7 @@
       <c r="J234" t="s">
         <v>1285</v>
       </c>
-      <c r="K234" t="s">
+      <c r="K234" s="3" t="s">
         <v>1286</v>
       </c>
       <c r="L234">
@@ -20759,7 +21191,7 @@
       <c r="J235" t="s">
         <v>1289</v>
       </c>
-      <c r="K235" t="s">
+      <c r="K235" s="3" t="s">
         <v>1290</v>
       </c>
       <c r="L235">
@@ -20821,7 +21253,7 @@
       <c r="J236" t="s">
         <v>1295</v>
       </c>
-      <c r="K236" t="s">
+      <c r="K236" s="3" t="s">
         <v>1296</v>
       </c>
       <c r="L236">
@@ -20883,7 +21315,7 @@
       <c r="J237" t="s">
         <v>1299</v>
       </c>
-      <c r="K237" t="s">
+      <c r="K237" s="3" t="s">
         <v>1300</v>
       </c>
       <c r="L237">
@@ -20945,7 +21377,7 @@
       <c r="J238" t="s">
         <v>1304</v>
       </c>
-      <c r="K238" t="s">
+      <c r="K238" s="3" t="s">
         <v>1305</v>
       </c>
       <c r="L238">
@@ -21010,7 +21442,7 @@
       <c r="J239" t="s">
         <v>1310</v>
       </c>
-      <c r="K239" t="s">
+      <c r="K239" s="3" t="s">
         <v>1311</v>
       </c>
       <c r="L239">
@@ -21078,7 +21510,7 @@
       <c r="J240" t="s">
         <v>1317</v>
       </c>
-      <c r="K240" t="s">
+      <c r="K240" s="3" t="s">
         <v>1318</v>
       </c>
       <c r="L240">
@@ -21140,7 +21572,7 @@
       <c r="J241" t="s">
         <v>1317</v>
       </c>
-      <c r="K241" t="s">
+      <c r="K241" s="3" t="s">
         <v>1322</v>
       </c>
       <c r="L241">
@@ -21205,7 +21637,7 @@
       <c r="I242" t="s">
         <v>1326</v>
       </c>
-      <c r="K242" t="s">
+      <c r="K242" s="3" t="s">
         <v>1327</v>
       </c>
       <c r="L242">
@@ -21273,7 +21705,7 @@
       <c r="J243" t="s">
         <v>1331</v>
       </c>
-      <c r="K243" t="s">
+      <c r="K243" s="3" t="s">
         <v>1332</v>
       </c>
       <c r="L243">
@@ -21332,7 +21764,7 @@
       <c r="J244" t="s">
         <v>1336</v>
       </c>
-      <c r="K244" t="s">
+      <c r="K244" s="3" t="s">
         <v>1337</v>
       </c>
       <c r="L244">
@@ -21394,7 +21826,7 @@
       <c r="J245" t="s">
         <v>1342</v>
       </c>
-      <c r="K245" t="s">
+      <c r="K245" s="3" t="s">
         <v>1343</v>
       </c>
       <c r="L245">
@@ -21456,7 +21888,7 @@
       <c r="J246" t="s">
         <v>1346</v>
       </c>
-      <c r="K246" t="s">
+      <c r="K246" s="3" t="s">
         <v>1347</v>
       </c>
       <c r="L246">
@@ -21524,7 +21956,7 @@
       <c r="J247" t="s">
         <v>1352</v>
       </c>
-      <c r="K247" t="s">
+      <c r="K247" s="3" t="s">
         <v>1353</v>
       </c>
       <c r="L247">
@@ -21583,7 +22015,7 @@
       <c r="I248" t="s">
         <v>1356</v>
       </c>
-      <c r="K248" t="s">
+      <c r="K248" s="3" t="s">
         <v>1357</v>
       </c>
       <c r="L248">
@@ -21651,7 +22083,7 @@
       <c r="J249" t="s">
         <v>1361</v>
       </c>
-      <c r="K249" t="s">
+      <c r="K249" s="3" t="s">
         <v>1362</v>
       </c>
       <c r="L249">
@@ -21719,7 +22151,7 @@
       <c r="J250" t="s">
         <v>1365</v>
       </c>
-      <c r="K250" t="s">
+      <c r="K250" s="3" t="s">
         <v>1366</v>
       </c>
       <c r="L250">
@@ -21781,7 +22213,7 @@
       <c r="J251" t="s">
         <v>1369</v>
       </c>
-      <c r="K251" t="s">
+      <c r="K251" s="3" t="s">
         <v>1370</v>
       </c>
       <c r="L251">
@@ -21840,7 +22272,7 @@
       <c r="I252" t="s">
         <v>1374</v>
       </c>
-      <c r="K252" t="s">
+      <c r="K252" s="3" t="s">
         <v>1375</v>
       </c>
       <c r="L252">
@@ -21902,7 +22334,7 @@
       <c r="J253" t="s">
         <v>1379</v>
       </c>
-      <c r="K253" t="s">
+      <c r="K253" s="3" t="s">
         <v>1380</v>
       </c>
       <c r="L253">
@@ -21964,7 +22396,7 @@
       <c r="J254" t="s">
         <v>1385</v>
       </c>
-      <c r="K254" t="s">
+      <c r="K254" s="3" t="s">
         <v>1386</v>
       </c>
       <c r="L254">
@@ -22026,7 +22458,7 @@
       <c r="J255" t="s">
         <v>1389</v>
       </c>
-      <c r="K255" t="s">
+      <c r="K255" s="3" t="s">
         <v>1390</v>
       </c>
       <c r="L255">
@@ -22088,7 +22520,7 @@
       <c r="J256" t="s">
         <v>1393</v>
       </c>
-      <c r="K256" t="s">
+      <c r="K256" s="3" t="s">
         <v>1394</v>
       </c>
       <c r="L256">
@@ -22156,7 +22588,7 @@
       <c r="J257" t="s">
         <v>1398</v>
       </c>
-      <c r="K257" t="s">
+      <c r="K257" s="3" t="s">
         <v>1399</v>
       </c>
       <c r="L257">
@@ -22218,7 +22650,7 @@
       <c r="J258" t="s">
         <v>1403</v>
       </c>
-      <c r="K258" t="s">
+      <c r="K258" s="3" t="s">
         <v>1404</v>
       </c>
       <c r="L258">
@@ -22280,7 +22712,7 @@
       <c r="J259" t="s">
         <v>1408</v>
       </c>
-      <c r="K259" t="s">
+      <c r="K259" s="3" t="s">
         <v>1409</v>
       </c>
       <c r="L259">
@@ -22342,7 +22774,7 @@
       <c r="J260" t="s">
         <v>1412</v>
       </c>
-      <c r="K260" t="s">
+      <c r="K260" s="3" t="s">
         <v>1413</v>
       </c>
       <c r="L260">
@@ -22404,7 +22836,7 @@
       <c r="J261" t="s">
         <v>1416</v>
       </c>
-      <c r="K261" t="s">
+      <c r="K261" s="3" t="s">
         <v>1417</v>
       </c>
       <c r="L261">
@@ -22463,7 +22895,7 @@
       <c r="J262" t="s">
         <v>1420</v>
       </c>
-      <c r="K262" t="s">
+      <c r="K262" s="3" t="s">
         <v>1421</v>
       </c>
       <c r="L262">
@@ -22528,7 +22960,7 @@
       <c r="J263" t="s">
         <v>1426</v>
       </c>
-      <c r="K263" t="s">
+      <c r="K263" s="3" t="s">
         <v>1427</v>
       </c>
       <c r="L263">
@@ -22587,7 +23019,7 @@
       <c r="J264" t="s">
         <v>1431</v>
       </c>
-      <c r="K264" t="s">
+      <c r="K264" s="3" t="s">
         <v>1432</v>
       </c>
       <c r="L264">
@@ -22652,7 +23084,7 @@
       <c r="J265" t="s">
         <v>1436</v>
       </c>
-      <c r="K265" t="s">
+      <c r="K265" s="3" t="s">
         <v>1437</v>
       </c>
       <c r="L265">
@@ -22711,7 +23143,7 @@
       <c r="J266" t="s">
         <v>1441</v>
       </c>
-      <c r="K266" t="s">
+      <c r="K266" s="3" t="s">
         <v>1442</v>
       </c>
       <c r="L266">
@@ -22773,7 +23205,7 @@
       <c r="J267" t="s">
         <v>1447</v>
       </c>
-      <c r="K267" t="s">
+      <c r="K267" s="3" t="s">
         <v>1448</v>
       </c>
       <c r="L267">
@@ -22832,7 +23264,7 @@
       <c r="J268" t="s">
         <v>1451</v>
       </c>
-      <c r="K268" t="s">
+      <c r="K268" s="3" t="s">
         <v>1452</v>
       </c>
       <c r="L268">
@@ -22894,7 +23326,7 @@
       <c r="J269" t="s">
         <v>1456</v>
       </c>
-      <c r="K269" t="s">
+      <c r="K269" s="3" t="s">
         <v>1457</v>
       </c>
       <c r="L269">
@@ -22953,7 +23385,7 @@
       <c r="J270" t="s">
         <v>1461</v>
       </c>
-      <c r="K270" t="s">
+      <c r="K270" s="3" t="s">
         <v>1462</v>
       </c>
       <c r="L270">
@@ -23015,7 +23447,7 @@
       <c r="J271" t="s">
         <v>1469</v>
       </c>
-      <c r="K271" t="s">
+      <c r="K271" s="3" t="s">
         <v>1470</v>
       </c>
       <c r="L271">
@@ -23077,7 +23509,7 @@
       <c r="J272" t="s">
         <v>1474</v>
       </c>
-      <c r="K272" t="s">
+      <c r="K272" s="3" t="s">
         <v>1475</v>
       </c>
       <c r="L272">
@@ -23139,7 +23571,7 @@
       <c r="J273" t="s">
         <v>1478</v>
       </c>
-      <c r="K273" t="s">
+      <c r="K273" s="3" t="s">
         <v>1479</v>
       </c>
       <c r="L273">
@@ -23198,7 +23630,7 @@
       <c r="J274" t="s">
         <v>1482</v>
       </c>
-      <c r="K274" t="s">
+      <c r="K274" s="3" t="s">
         <v>1483</v>
       </c>
       <c r="L274">
@@ -23257,7 +23689,7 @@
       <c r="J275" t="s">
         <v>1487</v>
       </c>
-      <c r="K275" t="s">
+      <c r="K275" s="3" t="s">
         <v>1488</v>
       </c>
       <c r="L275">
@@ -23325,7 +23757,7 @@
       <c r="J276" t="s">
         <v>1492</v>
       </c>
-      <c r="K276" t="s">
+      <c r="K276" s="3" t="s">
         <v>1493</v>
       </c>
       <c r="L276">
@@ -23387,7 +23819,7 @@
       <c r="J277" t="s">
         <v>1496</v>
       </c>
-      <c r="K277" t="s">
+      <c r="K277" s="3" t="s">
         <v>1497</v>
       </c>
       <c r="L277">
@@ -23455,7 +23887,7 @@
       <c r="J278" t="s">
         <v>1501</v>
       </c>
-      <c r="K278" t="s">
+      <c r="K278" s="3" t="s">
         <v>1502</v>
       </c>
       <c r="L278">
@@ -23517,7 +23949,7 @@
       <c r="J279" t="s">
         <v>1505</v>
       </c>
-      <c r="K279" t="s">
+      <c r="K279" s="3" t="s">
         <v>1506</v>
       </c>
       <c r="L279">
@@ -23573,7 +24005,7 @@
       <c r="J280" t="s">
         <v>1508</v>
       </c>
-      <c r="K280" t="s">
+      <c r="K280" s="3" t="s">
         <v>1509</v>
       </c>
       <c r="L280">
@@ -23632,7 +24064,7 @@
       <c r="J281" t="s">
         <v>1513</v>
       </c>
-      <c r="K281" t="s">
+      <c r="K281" s="3" t="s">
         <v>1514</v>
       </c>
       <c r="L281">
@@ -23694,7 +24126,7 @@
       <c r="J282" t="s">
         <v>1518</v>
       </c>
-      <c r="K282" t="s">
+      <c r="K282" s="3" t="s">
         <v>1519</v>
       </c>
       <c r="L282">
@@ -23759,7 +24191,7 @@
       <c r="J283" t="s">
         <v>1524</v>
       </c>
-      <c r="K283" t="s">
+      <c r="K283" s="3" t="s">
         <v>1525</v>
       </c>
       <c r="L283">
@@ -23821,7 +24253,7 @@
       <c r="J284" t="s">
         <v>1528</v>
       </c>
-      <c r="K284" t="s">
+      <c r="K284" s="3" t="s">
         <v>1529</v>
       </c>
       <c r="L284">
@@ -23849,7 +24281,7 @@
         <v>1531</v>
       </c>
       <c r="Y284" s="2" t="s">
-        <v>50</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="285" spans="2:25" x14ac:dyDescent="0.35">
@@ -23880,7 +24312,7 @@
       <c r="J285" t="s">
         <v>1532</v>
       </c>
-      <c r="K285" t="s">
+      <c r="K285" s="3" t="s">
         <v>1533</v>
       </c>
       <c r="L285">
@@ -23939,7 +24371,7 @@
       <c r="J286" t="s">
         <v>990</v>
       </c>
-      <c r="K286" t="s">
+      <c r="K286" s="3" t="s">
         <v>1536</v>
       </c>
       <c r="L286">
@@ -23998,7 +24430,7 @@
       <c r="J287" t="s">
         <v>1541</v>
       </c>
-      <c r="K287" t="s">
+      <c r="K287" s="3" t="s">
         <v>1542</v>
       </c>
       <c r="L287">
@@ -24060,7 +24492,7 @@
       <c r="J288" t="s">
         <v>1545</v>
       </c>
-      <c r="K288" t="s">
+      <c r="K288" s="3" t="s">
         <v>1546</v>
       </c>
       <c r="L288">
@@ -24122,7 +24554,7 @@
       <c r="J289" t="s">
         <v>1550</v>
       </c>
-      <c r="K289" t="s">
+      <c r="K289" s="3" t="s">
         <v>1551</v>
       </c>
       <c r="L289">
@@ -24184,7 +24616,7 @@
       <c r="J290" t="s">
         <v>1555</v>
       </c>
-      <c r="K290" t="s">
+      <c r="K290" s="3" t="s">
         <v>1556</v>
       </c>
       <c r="L290">
@@ -24246,7 +24678,7 @@
       <c r="J291" t="s">
         <v>1559</v>
       </c>
-      <c r="K291" t="s">
+      <c r="K291" s="3" t="s">
         <v>1560</v>
       </c>
       <c r="L291">
@@ -24308,7 +24740,7 @@
       <c r="J292" t="s">
         <v>1564</v>
       </c>
-      <c r="K292" t="s">
+      <c r="K292" s="3" t="s">
         <v>1565</v>
       </c>
       <c r="L292">
@@ -24370,7 +24802,7 @@
       <c r="J293" t="s">
         <v>1568</v>
       </c>
-      <c r="K293" t="s">
+      <c r="K293" s="3" t="s">
         <v>1569</v>
       </c>
       <c r="L293">
@@ -24426,7 +24858,7 @@
       <c r="I294" t="s">
         <v>1572</v>
       </c>
-      <c r="K294" t="s">
+      <c r="K294" s="3" t="s">
         <v>1573</v>
       </c>
       <c r="L294">
@@ -24494,7 +24926,7 @@
       <c r="J295" t="s">
         <v>1577</v>
       </c>
-      <c r="K295" t="s">
+      <c r="K295" s="3" t="s">
         <v>1578</v>
       </c>
       <c r="L295">
@@ -24553,7 +24985,7 @@
       <c r="J296" t="s">
         <v>1581</v>
       </c>
-      <c r="K296" t="s">
+      <c r="K296" s="3" t="s">
         <v>1582</v>
       </c>
       <c r="L296">
@@ -24612,7 +25044,7 @@
       <c r="J297" t="s">
         <v>1586</v>
       </c>
-      <c r="K297" t="s">
+      <c r="K297" s="3" t="s">
         <v>1587</v>
       </c>
       <c r="L297">
@@ -24671,7 +25103,7 @@
       <c r="J298" t="s">
         <v>1591</v>
       </c>
-      <c r="K298" t="s">
+      <c r="K298" s="3" t="s">
         <v>1592</v>
       </c>
       <c r="L298">
@@ -24736,7 +25168,7 @@
       <c r="J299" t="s">
         <v>1598</v>
       </c>
-      <c r="K299" t="s">
+      <c r="K299" s="3" t="s">
         <v>1599</v>
       </c>
       <c r="L299">
@@ -24795,7 +25227,7 @@
       <c r="I300" t="s">
         <v>720</v>
       </c>
-      <c r="K300" t="s">
+      <c r="K300" s="3" t="s">
         <v>1602</v>
       </c>
       <c r="L300">
@@ -24857,7 +25289,7 @@
       <c r="J301" t="s">
         <v>1607</v>
       </c>
-      <c r="K301" t="s">
+      <c r="K301" s="3" t="s">
         <v>1608</v>
       </c>
       <c r="L301">
@@ -24919,7 +25351,7 @@
       <c r="J302" t="s">
         <v>1611</v>
       </c>
-      <c r="K302" t="s">
+      <c r="K302" s="3" t="s">
         <v>1612</v>
       </c>
       <c r="L302">
@@ -24984,7 +25416,7 @@
       <c r="J303" t="s">
         <v>1619</v>
       </c>
-      <c r="K303" t="s">
+      <c r="K303" s="3" t="s">
         <v>1620</v>
       </c>
       <c r="L303">
@@ -25046,7 +25478,7 @@
       <c r="J304" t="s">
         <v>1624</v>
       </c>
-      <c r="K304" t="s">
+      <c r="K304" s="3" t="s">
         <v>1625</v>
       </c>
       <c r="L304">
@@ -25108,7 +25540,7 @@
       <c r="J305" t="s">
         <v>1629</v>
       </c>
-      <c r="K305" t="s">
+      <c r="K305" s="3" t="s">
         <v>1630</v>
       </c>
       <c r="L305">
@@ -25176,7 +25608,7 @@
       <c r="J306" t="s">
         <v>1636</v>
       </c>
-      <c r="K306" t="s">
+      <c r="K306" s="3" t="s">
         <v>1637</v>
       </c>
       <c r="L306">
@@ -25238,7 +25670,7 @@
       <c r="J307" t="s">
         <v>1640</v>
       </c>
-      <c r="K307" t="s">
+      <c r="K307" s="3" t="s">
         <v>1641</v>
       </c>
       <c r="L307">
@@ -25297,7 +25729,7 @@
       <c r="I308" t="s">
         <v>1645</v>
       </c>
-      <c r="K308" t="s">
+      <c r="K308" s="3" t="s">
         <v>1646</v>
       </c>
       <c r="L308">
@@ -26598,7 +27030,7 @@
       <c r="F330" t="s">
         <v>1749</v>
       </c>
-      <c r="K330" t="s">
+      <c r="K330" s="3" t="s">
         <v>1750</v>
       </c>
       <c r="N330">
@@ -27265,7 +27697,6 @@
       <c r="J341" t="s">
         <v>1815</v>
       </c>
-      <c r="K341" s="3"/>
       <c r="N341">
         <v>2009</v>
       </c>
@@ -28045,6 +28476,1417 @@
       </c>
       <c r="Y353" s="2" t="s">
         <v>1885</v>
+      </c>
+    </row>
+    <row r="354" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B354" t="s">
+        <v>1888</v>
+      </c>
+      <c r="C354" t="s">
+        <v>1889</v>
+      </c>
+      <c r="D354" t="s">
+        <v>27</v>
+      </c>
+      <c r="E354" t="s">
+        <v>28</v>
+      </c>
+      <c r="F354" t="s">
+        <v>29</v>
+      </c>
+      <c r="G354" t="s">
+        <v>30</v>
+      </c>
+      <c r="H354" t="s">
+        <v>144</v>
+      </c>
+      <c r="I354" t="s">
+        <v>426</v>
+      </c>
+      <c r="J354" t="s">
+        <v>1890</v>
+      </c>
+      <c r="K354" s="3" t="s">
+        <v>1891</v>
+      </c>
+      <c r="L354">
+        <v>48.854602300000003</v>
+      </c>
+      <c r="M354">
+        <v>2.482594598748042</v>
+      </c>
+      <c r="N354">
+        <v>2003</v>
+      </c>
+      <c r="O354">
+        <v>9</v>
+      </c>
+      <c r="P354">
+        <v>11</v>
+      </c>
+      <c r="Q354" t="s">
+        <v>183</v>
+      </c>
+      <c r="R354" t="s">
+        <v>1892</v>
+      </c>
+      <c r="S354" t="s">
+        <v>37</v>
+      </c>
+      <c r="V354">
+        <v>1</v>
+      </c>
+      <c r="W354" s="2" t="s">
+        <v>1893</v>
+      </c>
+      <c r="X354" s="2" t="s">
+        <v>1894</v>
+      </c>
+      <c r="Y354" s="2" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="355" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B355" t="s">
+        <v>93</v>
+      </c>
+      <c r="C355" t="s">
+        <v>26</v>
+      </c>
+      <c r="D355" t="s">
+        <v>27</v>
+      </c>
+      <c r="E355" t="s">
+        <v>28</v>
+      </c>
+      <c r="F355" t="s">
+        <v>29</v>
+      </c>
+      <c r="G355" t="s">
+        <v>30</v>
+      </c>
+      <c r="H355" t="s">
+        <v>31</v>
+      </c>
+      <c r="I355" t="s">
+        <v>1896</v>
+      </c>
+      <c r="J355" t="s">
+        <v>193</v>
+      </c>
+      <c r="K355" s="3" t="s">
+        <v>1897</v>
+      </c>
+      <c r="L355">
+        <v>48.870604999999998</v>
+      </c>
+      <c r="M355">
+        <v>2.4580299999999999</v>
+      </c>
+      <c r="N355">
+        <v>2008</v>
+      </c>
+      <c r="O355">
+        <v>6</v>
+      </c>
+      <c r="Q355" t="s">
+        <v>47</v>
+      </c>
+      <c r="R355" t="s">
+        <v>1898</v>
+      </c>
+      <c r="S355" t="s">
+        <v>37</v>
+      </c>
+      <c r="V355">
+        <v>1</v>
+      </c>
+      <c r="W355" s="2" t="s">
+        <v>1899</v>
+      </c>
+      <c r="X355" s="2" t="s">
+        <v>1900</v>
+      </c>
+      <c r="Y355" s="2" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="356" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B356" t="s">
+        <v>449</v>
+      </c>
+      <c r="C356" t="s">
+        <v>26</v>
+      </c>
+      <c r="D356" t="s">
+        <v>27</v>
+      </c>
+      <c r="E356" t="s">
+        <v>28</v>
+      </c>
+      <c r="F356" t="s">
+        <v>29</v>
+      </c>
+      <c r="G356" t="s">
+        <v>30</v>
+      </c>
+      <c r="H356" t="s">
+        <v>138</v>
+      </c>
+      <c r="I356" t="s">
+        <v>409</v>
+      </c>
+      <c r="J356" t="s">
+        <v>1902</v>
+      </c>
+      <c r="K356" s="3" t="s">
+        <v>1903</v>
+      </c>
+      <c r="L356">
+        <v>48.70987075</v>
+      </c>
+      <c r="M356">
+        <v>2.3790730644339622</v>
+      </c>
+      <c r="N356">
+        <v>2008</v>
+      </c>
+      <c r="O356">
+        <v>5</v>
+      </c>
+      <c r="Q356" t="s">
+        <v>47</v>
+      </c>
+      <c r="R356" t="s">
+        <v>1904</v>
+      </c>
+      <c r="S356" t="s">
+        <v>37</v>
+      </c>
+      <c r="V356">
+        <v>1</v>
+      </c>
+      <c r="W356" s="2" t="s">
+        <v>1905</v>
+      </c>
+      <c r="X356" s="2" t="s">
+        <v>1906</v>
+      </c>
+      <c r="Y356" s="2" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="357" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B357" t="s">
+        <v>1789</v>
+      </c>
+      <c r="C357" t="s">
+        <v>1790</v>
+      </c>
+      <c r="D357" t="s">
+        <v>27</v>
+      </c>
+      <c r="E357" t="s">
+        <v>28</v>
+      </c>
+      <c r="F357" t="s">
+        <v>29</v>
+      </c>
+      <c r="G357" t="s">
+        <v>30</v>
+      </c>
+      <c r="H357" t="s">
+        <v>356</v>
+      </c>
+      <c r="I357" t="s">
+        <v>583</v>
+      </c>
+      <c r="J357" t="s">
+        <v>1908</v>
+      </c>
+      <c r="K357" s="3" t="s">
+        <v>1909</v>
+      </c>
+      <c r="L357">
+        <v>48.924676400000003</v>
+      </c>
+      <c r="M357">
+        <v>2.1829898000000001</v>
+      </c>
+      <c r="N357">
+        <v>2008</v>
+      </c>
+      <c r="O357">
+        <v>6</v>
+      </c>
+      <c r="Q357" t="s">
+        <v>47</v>
+      </c>
+      <c r="V357">
+        <v>1</v>
+      </c>
+      <c r="W357" s="2" t="s">
+        <v>1910</v>
+      </c>
+      <c r="X357" s="2" t="s">
+        <v>1911</v>
+      </c>
+      <c r="Y357" s="2" t="s">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="358" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B358" t="s">
+        <v>1913</v>
+      </c>
+      <c r="C358" t="s">
+        <v>1914</v>
+      </c>
+      <c r="D358" t="s">
+        <v>27</v>
+      </c>
+      <c r="E358" t="s">
+        <v>28</v>
+      </c>
+      <c r="F358" t="s">
+        <v>29</v>
+      </c>
+      <c r="G358" t="s">
+        <v>30</v>
+      </c>
+      <c r="H358" t="s">
+        <v>144</v>
+      </c>
+      <c r="I358" t="s">
+        <v>145</v>
+      </c>
+      <c r="J358" t="s">
+        <v>1915</v>
+      </c>
+      <c r="N358">
+        <v>1993</v>
+      </c>
+      <c r="O358">
+        <v>9</v>
+      </c>
+      <c r="P358">
+        <v>11</v>
+      </c>
+      <c r="Q358" t="s">
+        <v>183</v>
+      </c>
+      <c r="R358" t="s">
+        <v>1916</v>
+      </c>
+      <c r="S358" t="s">
+        <v>37</v>
+      </c>
+      <c r="V358">
+        <v>0</v>
+      </c>
+      <c r="Y358" s="2" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="359" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B359" t="s">
+        <v>1913</v>
+      </c>
+      <c r="C359" t="s">
+        <v>1914</v>
+      </c>
+      <c r="D359" t="s">
+        <v>27</v>
+      </c>
+      <c r="E359" t="s">
+        <v>28</v>
+      </c>
+      <c r="F359" t="s">
+        <v>29</v>
+      </c>
+      <c r="G359" t="s">
+        <v>51</v>
+      </c>
+      <c r="H359" t="s">
+        <v>52</v>
+      </c>
+      <c r="I359" t="s">
+        <v>53</v>
+      </c>
+      <c r="J359" t="s">
+        <v>1918</v>
+      </c>
+      <c r="K359" s="3">
+        <v>45140</v>
+      </c>
+      <c r="N359">
+        <v>2006</v>
+      </c>
+      <c r="Q359" t="s">
+        <v>704</v>
+      </c>
+      <c r="R359" t="s">
+        <v>1919</v>
+      </c>
+      <c r="S359" t="s">
+        <v>37</v>
+      </c>
+      <c r="V359">
+        <v>0</v>
+      </c>
+      <c r="W359" s="2" t="s">
+        <v>1920</v>
+      </c>
+      <c r="X359" s="2" t="s">
+        <v>1921</v>
+      </c>
+      <c r="Y359" s="2" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="360" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B360" t="s">
+        <v>1923</v>
+      </c>
+      <c r="C360" t="s">
+        <v>1790</v>
+      </c>
+      <c r="D360" t="s">
+        <v>27</v>
+      </c>
+      <c r="E360" t="s">
+        <v>28</v>
+      </c>
+      <c r="F360" t="s">
+        <v>29</v>
+      </c>
+      <c r="G360" t="s">
+        <v>61</v>
+      </c>
+      <c r="H360" t="s">
+        <v>725</v>
+      </c>
+      <c r="I360" t="s">
+        <v>726</v>
+      </c>
+      <c r="J360" t="s">
+        <v>1924</v>
+      </c>
+      <c r="N360">
+        <v>2008</v>
+      </c>
+      <c r="O360">
+        <v>11</v>
+      </c>
+      <c r="P360">
+        <v>22</v>
+      </c>
+      <c r="Q360" t="s">
+        <v>35</v>
+      </c>
+      <c r="V360">
+        <v>0</v>
+      </c>
+      <c r="X360" s="2" t="s">
+        <v>1925</v>
+      </c>
+      <c r="Y360" s="2" t="s">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="361" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B361" t="s">
+        <v>1927</v>
+      </c>
+      <c r="C361" t="s">
+        <v>26</v>
+      </c>
+      <c r="D361" t="s">
+        <v>27</v>
+      </c>
+      <c r="E361" t="s">
+        <v>28</v>
+      </c>
+      <c r="F361" t="s">
+        <v>29</v>
+      </c>
+      <c r="G361" t="s">
+        <v>30</v>
+      </c>
+      <c r="H361" t="s">
+        <v>431</v>
+      </c>
+      <c r="I361" t="s">
+        <v>432</v>
+      </c>
+      <c r="K361" s="3">
+        <v>95100</v>
+      </c>
+      <c r="L361">
+        <v>48.942990000000002</v>
+      </c>
+      <c r="M361">
+        <v>2.2498200000000002</v>
+      </c>
+      <c r="N361">
+        <v>1973</v>
+      </c>
+      <c r="O361">
+        <v>9</v>
+      </c>
+      <c r="P361">
+        <v>14</v>
+      </c>
+      <c r="Q361" t="s">
+        <v>704</v>
+      </c>
+      <c r="R361" t="s">
+        <v>1928</v>
+      </c>
+      <c r="S361" t="s">
+        <v>37</v>
+      </c>
+      <c r="V361">
+        <v>1</v>
+      </c>
+      <c r="W361" s="2" t="s">
+        <v>1929</v>
+      </c>
+      <c r="X361" s="2" t="s">
+        <v>1930</v>
+      </c>
+      <c r="Y361" s="2" t="s">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="362" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B362" t="s">
+        <v>60</v>
+      </c>
+      <c r="C362" t="s">
+        <v>26</v>
+      </c>
+      <c r="D362" t="s">
+        <v>27</v>
+      </c>
+      <c r="E362" t="s">
+        <v>28</v>
+      </c>
+      <c r="F362" t="s">
+        <v>29</v>
+      </c>
+      <c r="G362" t="s">
+        <v>30</v>
+      </c>
+      <c r="H362" t="s">
+        <v>31</v>
+      </c>
+      <c r="I362" t="s">
+        <v>32</v>
+      </c>
+      <c r="J362" t="s">
+        <v>1932</v>
+      </c>
+      <c r="K362" s="3" t="s">
+        <v>1933</v>
+      </c>
+      <c r="L362">
+        <v>48.946370199999997</v>
+      </c>
+      <c r="M362">
+        <v>2.3851605</v>
+      </c>
+      <c r="N362">
+        <v>2008</v>
+      </c>
+      <c r="O362">
+        <v>9</v>
+      </c>
+      <c r="P362">
+        <v>19</v>
+      </c>
+      <c r="Q362" t="s">
+        <v>35</v>
+      </c>
+      <c r="V362">
+        <v>1</v>
+      </c>
+      <c r="W362" s="2" t="s">
+        <v>1934</v>
+      </c>
+      <c r="X362" s="2" t="s">
+        <v>1935</v>
+      </c>
+      <c r="Y362" s="2" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="363" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B363" t="s">
+        <v>114</v>
+      </c>
+      <c r="C363" t="s">
+        <v>26</v>
+      </c>
+      <c r="D363" t="s">
+        <v>27</v>
+      </c>
+      <c r="E363" t="s">
+        <v>28</v>
+      </c>
+      <c r="F363" t="s">
+        <v>29</v>
+      </c>
+      <c r="G363" t="s">
+        <v>30</v>
+      </c>
+      <c r="H363" t="s">
+        <v>31</v>
+      </c>
+      <c r="I363" t="s">
+        <v>415</v>
+      </c>
+      <c r="J363" t="s">
+        <v>1937</v>
+      </c>
+      <c r="K363" s="3" t="s">
+        <v>1938</v>
+      </c>
+      <c r="L363">
+        <v>48.959560799999998</v>
+      </c>
+      <c r="M363">
+        <v>2.5670727000000002</v>
+      </c>
+      <c r="N363">
+        <v>2008</v>
+      </c>
+      <c r="O363">
+        <v>6</v>
+      </c>
+      <c r="Q363" t="s">
+        <v>47</v>
+      </c>
+      <c r="V363">
+        <v>1</v>
+      </c>
+      <c r="W363" s="2" t="s">
+        <v>1939</v>
+      </c>
+      <c r="X363" s="2" t="s">
+        <v>1940</v>
+      </c>
+      <c r="Y363" s="2" t="s">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="364" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B364" t="s">
+        <v>1942</v>
+      </c>
+      <c r="C364" t="s">
+        <v>26</v>
+      </c>
+      <c r="D364" t="s">
+        <v>27</v>
+      </c>
+      <c r="E364" t="s">
+        <v>28</v>
+      </c>
+      <c r="F364" t="s">
+        <v>29</v>
+      </c>
+      <c r="G364" t="s">
+        <v>30</v>
+      </c>
+      <c r="H364" t="s">
+        <v>1014</v>
+      </c>
+      <c r="I364" t="s">
+        <v>1775</v>
+      </c>
+      <c r="J364" t="s">
+        <v>1776</v>
+      </c>
+      <c r="K364" s="3" t="s">
+        <v>1777</v>
+      </c>
+      <c r="L364">
+        <v>48.763906800000001</v>
+      </c>
+      <c r="M364">
+        <v>2.2719914000000001</v>
+      </c>
+      <c r="N364">
+        <v>2008</v>
+      </c>
+      <c r="O364">
+        <v>6</v>
+      </c>
+      <c r="Q364" t="s">
+        <v>47</v>
+      </c>
+      <c r="V364">
+        <v>1</v>
+      </c>
+      <c r="W364" s="2" t="s">
+        <v>1943</v>
+      </c>
+      <c r="X364" s="2" t="s">
+        <v>1944</v>
+      </c>
+      <c r="Y364" s="2" t="s">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="365" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B365" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C365" t="s">
+        <v>450</v>
+      </c>
+      <c r="D365" t="s">
+        <v>27</v>
+      </c>
+      <c r="E365" t="s">
+        <v>28</v>
+      </c>
+      <c r="F365" t="s">
+        <v>29</v>
+      </c>
+      <c r="G365" t="s">
+        <v>100</v>
+      </c>
+      <c r="H365" t="s">
+        <v>663</v>
+      </c>
+      <c r="I365" t="s">
+        <v>1946</v>
+      </c>
+      <c r="J365" t="s">
+        <v>1947</v>
+      </c>
+      <c r="L365">
+        <v>48.098597050000002</v>
+      </c>
+      <c r="M365">
+        <v>-1.705740089891044</v>
+      </c>
+      <c r="N365">
+        <v>2008</v>
+      </c>
+      <c r="O365">
+        <v>9</v>
+      </c>
+      <c r="P365">
+        <v>5</v>
+      </c>
+      <c r="Q365" t="s">
+        <v>35</v>
+      </c>
+      <c r="V365">
+        <v>1</v>
+      </c>
+      <c r="W365" s="2" t="s">
+        <v>1948</v>
+      </c>
+      <c r="X365" s="2" t="s">
+        <v>1949</v>
+      </c>
+      <c r="Y365" s="2" t="s">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="366" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B366" t="s">
+        <v>449</v>
+      </c>
+      <c r="C366" t="s">
+        <v>26</v>
+      </c>
+      <c r="D366" t="s">
+        <v>27</v>
+      </c>
+      <c r="E366" t="s">
+        <v>28</v>
+      </c>
+      <c r="F366" t="s">
+        <v>29</v>
+      </c>
+      <c r="G366" t="s">
+        <v>30</v>
+      </c>
+      <c r="H366" t="s">
+        <v>31</v>
+      </c>
+      <c r="I366" t="s">
+        <v>193</v>
+      </c>
+      <c r="J366" t="s">
+        <v>1951</v>
+      </c>
+      <c r="K366" s="3" t="s">
+        <v>1952</v>
+      </c>
+      <c r="L366">
+        <v>48.8786427</v>
+      </c>
+      <c r="M366">
+        <v>2.4493377999999999</v>
+      </c>
+      <c r="N366">
+        <v>2008</v>
+      </c>
+      <c r="O366">
+        <v>9</v>
+      </c>
+      <c r="P366">
+        <v>1</v>
+      </c>
+      <c r="Q366" t="s">
+        <v>35</v>
+      </c>
+      <c r="V366">
+        <v>1</v>
+      </c>
+      <c r="W366" s="2" t="s">
+        <v>1953</v>
+      </c>
+      <c r="X366" s="2" t="s">
+        <v>1954</v>
+      </c>
+      <c r="Y366" s="2" t="s">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="367" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B367" t="s">
+        <v>449</v>
+      </c>
+      <c r="C367" t="s">
+        <v>450</v>
+      </c>
+      <c r="D367" t="s">
+        <v>27</v>
+      </c>
+      <c r="E367" t="s">
+        <v>28</v>
+      </c>
+      <c r="F367" t="s">
+        <v>29</v>
+      </c>
+      <c r="G367" t="s">
+        <v>30</v>
+      </c>
+      <c r="H367" t="s">
+        <v>31</v>
+      </c>
+      <c r="I367" t="s">
+        <v>193</v>
+      </c>
+      <c r="J367" t="s">
+        <v>1956</v>
+      </c>
+      <c r="K367" s="3" t="s">
+        <v>1957</v>
+      </c>
+      <c r="L367">
+        <v>48.868476450000003</v>
+      </c>
+      <c r="M367">
+        <v>2.417216450753028</v>
+      </c>
+      <c r="N367">
+        <v>1973</v>
+      </c>
+      <c r="O367">
+        <v>10</v>
+      </c>
+      <c r="P367">
+        <v>27</v>
+      </c>
+      <c r="Q367" t="s">
+        <v>183</v>
+      </c>
+      <c r="R367" t="s">
+        <v>1958</v>
+      </c>
+      <c r="S367" t="s">
+        <v>37</v>
+      </c>
+      <c r="V367">
+        <v>1</v>
+      </c>
+      <c r="W367" s="2" t="s">
+        <v>1959</v>
+      </c>
+      <c r="X367" s="2" t="s">
+        <v>1960</v>
+      </c>
+      <c r="Y367" s="2" t="s">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="368" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B368" t="s">
+        <v>1962</v>
+      </c>
+      <c r="C368" t="s">
+        <v>26</v>
+      </c>
+      <c r="D368" t="s">
+        <v>27</v>
+      </c>
+      <c r="E368" t="s">
+        <v>28</v>
+      </c>
+      <c r="F368" t="s">
+        <v>29</v>
+      </c>
+      <c r="G368" t="s">
+        <v>30</v>
+      </c>
+      <c r="H368" t="s">
+        <v>31</v>
+      </c>
+      <c r="I368" t="s">
+        <v>415</v>
+      </c>
+      <c r="J368" t="s">
+        <v>1963</v>
+      </c>
+      <c r="K368" s="3" t="s">
+        <v>1964</v>
+      </c>
+      <c r="L368">
+        <v>48.9110814</v>
+      </c>
+      <c r="M368">
+        <v>2.5165278</v>
+      </c>
+      <c r="N368">
+        <v>2008</v>
+      </c>
+      <c r="O368">
+        <v>6</v>
+      </c>
+      <c r="Q368" t="s">
+        <v>47</v>
+      </c>
+      <c r="R368" t="s">
+        <v>1965</v>
+      </c>
+      <c r="S368" t="s">
+        <v>37</v>
+      </c>
+      <c r="V368">
+        <v>1</v>
+      </c>
+      <c r="W368" s="2" t="s">
+        <v>1966</v>
+      </c>
+      <c r="X368" s="2" t="s">
+        <v>1967</v>
+      </c>
+      <c r="Y368" s="2" t="s">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="369" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B369" t="s">
+        <v>449</v>
+      </c>
+      <c r="C369" t="s">
+        <v>450</v>
+      </c>
+      <c r="D369" t="s">
+        <v>27</v>
+      </c>
+      <c r="E369" t="s">
+        <v>28</v>
+      </c>
+      <c r="F369" t="s">
+        <v>29</v>
+      </c>
+      <c r="G369" t="s">
+        <v>30</v>
+      </c>
+      <c r="H369" t="s">
+        <v>144</v>
+      </c>
+      <c r="I369" t="s">
+        <v>1809</v>
+      </c>
+      <c r="J369" t="s">
+        <v>1969</v>
+      </c>
+      <c r="K369" s="3">
+        <v>94000</v>
+      </c>
+      <c r="L369">
+        <v>48.779213968870202</v>
+      </c>
+      <c r="M369">
+        <v>2.4530095890300401</v>
+      </c>
+      <c r="N369">
+        <v>2008</v>
+      </c>
+      <c r="O369">
+        <v>8</v>
+      </c>
+      <c r="P369">
+        <v>25</v>
+      </c>
+      <c r="Q369" t="s">
+        <v>35</v>
+      </c>
+      <c r="V369">
+        <v>1</v>
+      </c>
+      <c r="W369" s="2" t="s">
+        <v>1970</v>
+      </c>
+      <c r="X369" s="2" t="s">
+        <v>1971</v>
+      </c>
+      <c r="Y369" s="2" t="s">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="370" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B370" t="s">
+        <v>644</v>
+      </c>
+      <c r="C370" t="s">
+        <v>26</v>
+      </c>
+      <c r="D370" t="s">
+        <v>27</v>
+      </c>
+      <c r="E370" t="s">
+        <v>28</v>
+      </c>
+      <c r="F370" t="s">
+        <v>1973</v>
+      </c>
+      <c r="G370" t="s">
+        <v>1974</v>
+      </c>
+      <c r="H370" t="s">
+        <v>1975</v>
+      </c>
+      <c r="K370" s="3" t="s">
+        <v>1976</v>
+      </c>
+      <c r="L370">
+        <v>16.421083500000002</v>
+      </c>
+      <c r="M370">
+        <v>-61.529373100000001</v>
+      </c>
+      <c r="N370">
+        <v>2008</v>
+      </c>
+      <c r="O370">
+        <v>8</v>
+      </c>
+      <c r="P370">
+        <v>25</v>
+      </c>
+      <c r="Q370" t="s">
+        <v>35</v>
+      </c>
+      <c r="V370">
+        <v>1</v>
+      </c>
+      <c r="W370" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="Y370" s="2" t="s">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="371" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B371" t="s">
+        <v>93</v>
+      </c>
+      <c r="C371" t="s">
+        <v>26</v>
+      </c>
+      <c r="D371" t="s">
+        <v>27</v>
+      </c>
+      <c r="E371" t="s">
+        <v>28</v>
+      </c>
+      <c r="F371" t="s">
+        <v>29</v>
+      </c>
+      <c r="G371" t="s">
+        <v>30</v>
+      </c>
+      <c r="H371" t="s">
+        <v>31</v>
+      </c>
+      <c r="I371" t="s">
+        <v>415</v>
+      </c>
+      <c r="J371" t="s">
+        <v>1979</v>
+      </c>
+      <c r="K371" s="3" t="s">
+        <v>1980</v>
+      </c>
+      <c r="L371">
+        <v>48.956343400000002</v>
+      </c>
+      <c r="M371">
+        <v>2.5494696000000001</v>
+      </c>
+      <c r="N371">
+        <v>2008</v>
+      </c>
+      <c r="O371">
+        <v>8</v>
+      </c>
+      <c r="P371">
+        <v>25</v>
+      </c>
+      <c r="Q371" t="s">
+        <v>35</v>
+      </c>
+      <c r="V371">
+        <v>1</v>
+      </c>
+      <c r="W371" s="2" t="s">
+        <v>1981</v>
+      </c>
+      <c r="X371" s="2" t="s">
+        <v>1982</v>
+      </c>
+      <c r="Y371" s="2" t="s">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="372" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B372" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C372" t="s">
+        <v>26</v>
+      </c>
+      <c r="D372" t="s">
+        <v>27</v>
+      </c>
+      <c r="E372" t="s">
+        <v>28</v>
+      </c>
+      <c r="F372" t="s">
+        <v>29</v>
+      </c>
+      <c r="G372" t="s">
+        <v>30</v>
+      </c>
+      <c r="H372" t="s">
+        <v>31</v>
+      </c>
+      <c r="I372" t="s">
+        <v>32</v>
+      </c>
+      <c r="J372" t="s">
+        <v>1985</v>
+      </c>
+      <c r="K372" s="3" t="s">
+        <v>1986</v>
+      </c>
+      <c r="L372">
+        <v>48.962346699999998</v>
+      </c>
+      <c r="M372">
+        <v>2.3619211</v>
+      </c>
+      <c r="N372">
+        <v>2008</v>
+      </c>
+      <c r="O372">
+        <v>7</v>
+      </c>
+      <c r="P372">
+        <v>24</v>
+      </c>
+      <c r="Q372" t="s">
+        <v>35</v>
+      </c>
+      <c r="V372">
+        <v>1</v>
+      </c>
+      <c r="W372" s="2" t="s">
+        <v>1987</v>
+      </c>
+      <c r="X372" s="2" t="s">
+        <v>1988</v>
+      </c>
+      <c r="Y372" s="2" t="s">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="373" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B373" t="s">
+        <v>449</v>
+      </c>
+      <c r="C373" t="s">
+        <v>450</v>
+      </c>
+      <c r="D373" t="s">
+        <v>27</v>
+      </c>
+      <c r="E373" t="s">
+        <v>28</v>
+      </c>
+      <c r="F373" t="s">
+        <v>29</v>
+      </c>
+      <c r="G373" t="s">
+        <v>30</v>
+      </c>
+      <c r="H373" t="s">
+        <v>31</v>
+      </c>
+      <c r="I373" t="s">
+        <v>193</v>
+      </c>
+      <c r="J373" t="s">
+        <v>1990</v>
+      </c>
+      <c r="K373" s="3" t="s">
+        <v>1991</v>
+      </c>
+      <c r="L373">
+        <v>48.897441950000001</v>
+      </c>
+      <c r="M373">
+        <v>2.400922160434487</v>
+      </c>
+      <c r="N373">
+        <v>2008</v>
+      </c>
+      <c r="O373">
+        <v>7</v>
+      </c>
+      <c r="P373">
+        <v>19</v>
+      </c>
+      <c r="Q373" t="s">
+        <v>35</v>
+      </c>
+      <c r="R373" t="s">
+        <v>1992</v>
+      </c>
+      <c r="S373" t="s">
+        <v>37</v>
+      </c>
+      <c r="V373">
+        <v>1</v>
+      </c>
+      <c r="W373" s="2" t="s">
+        <v>1993</v>
+      </c>
+      <c r="X373" s="2" t="s">
+        <v>1994</v>
+      </c>
+      <c r="Y373" s="2" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="374" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B374" t="s">
+        <v>1996</v>
+      </c>
+      <c r="C374" t="s">
+        <v>741</v>
+      </c>
+      <c r="D374" t="s">
+        <v>27</v>
+      </c>
+      <c r="E374" t="s">
+        <v>28</v>
+      </c>
+      <c r="F374" t="s">
+        <v>29</v>
+      </c>
+      <c r="G374" t="s">
+        <v>30</v>
+      </c>
+      <c r="H374" t="s">
+        <v>138</v>
+      </c>
+      <c r="I374" t="s">
+        <v>409</v>
+      </c>
+      <c r="J374" t="s">
+        <v>1997</v>
+      </c>
+      <c r="K374" s="3" t="s">
+        <v>1998</v>
+      </c>
+      <c r="L374">
+        <v>48.683364699999998</v>
+      </c>
+      <c r="M374">
+        <v>2.3377005</v>
+      </c>
+      <c r="N374">
+        <v>2008</v>
+      </c>
+      <c r="O374">
+        <v>7</v>
+      </c>
+      <c r="P374">
+        <v>8</v>
+      </c>
+      <c r="Q374" t="s">
+        <v>35</v>
+      </c>
+      <c r="V374">
+        <v>1</v>
+      </c>
+      <c r="W374" s="2" t="s">
+        <v>1999</v>
+      </c>
+      <c r="X374" s="2" t="s">
+        <v>2000</v>
+      </c>
+      <c r="Y374" s="2" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="375" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B375" t="s">
+        <v>114</v>
+      </c>
+      <c r="C375" t="s">
+        <v>26</v>
+      </c>
+      <c r="D375" t="s">
+        <v>27</v>
+      </c>
+      <c r="E375" t="s">
+        <v>28</v>
+      </c>
+      <c r="F375" t="s">
+        <v>29</v>
+      </c>
+      <c r="G375" t="s">
+        <v>30</v>
+      </c>
+      <c r="H375" t="s">
+        <v>138</v>
+      </c>
+      <c r="I375" t="s">
+        <v>2002</v>
+      </c>
+      <c r="J375" t="s">
+        <v>139</v>
+      </c>
+      <c r="K375" s="3" t="s">
+        <v>2003</v>
+      </c>
+      <c r="L375">
+        <v>48.660161299999999</v>
+      </c>
+      <c r="M375">
+        <v>2.3481809</v>
+      </c>
+      <c r="N375">
+        <v>2008</v>
+      </c>
+      <c r="O375">
+        <v>7</v>
+      </c>
+      <c r="P375">
+        <v>6</v>
+      </c>
+      <c r="Q375" t="s">
+        <v>35</v>
+      </c>
+      <c r="V375">
+        <v>1</v>
+      </c>
+      <c r="W375" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="X375" s="2" t="s">
+        <v>2005</v>
+      </c>
+      <c r="Y375" s="2" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="376" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B376" t="s">
+        <v>60</v>
+      </c>
+      <c r="C376" t="s">
+        <v>26</v>
+      </c>
+      <c r="D376" t="s">
+        <v>27</v>
+      </c>
+      <c r="E376" t="s">
+        <v>28</v>
+      </c>
+      <c r="F376" t="s">
+        <v>29</v>
+      </c>
+      <c r="G376" t="s">
+        <v>30</v>
+      </c>
+      <c r="H376" t="s">
+        <v>1014</v>
+      </c>
+      <c r="I376" t="s">
+        <v>1775</v>
+      </c>
+      <c r="J376" t="s">
+        <v>2007</v>
+      </c>
+      <c r="K376" s="3" t="s">
+        <v>2008</v>
+      </c>
+      <c r="L376">
+        <v>48.820548199999998</v>
+      </c>
+      <c r="M376">
+        <v>2.3039147999999998</v>
+      </c>
+      <c r="N376">
+        <v>2008</v>
+      </c>
+      <c r="O376">
+        <v>5</v>
+      </c>
+      <c r="Q376" t="s">
+        <v>47</v>
+      </c>
+      <c r="R376" t="s">
+        <v>2009</v>
+      </c>
+      <c r="S376" t="s">
+        <v>37</v>
+      </c>
+      <c r="V376">
+        <v>1</v>
+      </c>
+      <c r="W376" s="2" t="s">
+        <v>2010</v>
+      </c>
+      <c r="X376" s="2" t="s">
+        <v>2011</v>
+      </c>
+      <c r="Y376" s="2" t="s">
+        <v>2012</v>
       </c>
     </row>
   </sheetData>
@@ -29093,6 +30935,71 @@
     <hyperlink ref="W353" r:id="rId1038" xr:uid="{62F1E038-B0F8-474A-9599-80B0394D3E07}"/>
     <hyperlink ref="Y353" r:id="rId1039" xr:uid="{1D84A01E-D74A-4529-9C03-55FE6767E7C5}"/>
     <hyperlink ref="X353" r:id="rId1040" xr:uid="{A57CDA93-9212-4A16-8B1B-8084B9257563}"/>
+    <hyperlink ref="W354" r:id="rId1041" xr:uid="{FA37490F-D01F-4C82-ACAA-9929DA68F9AD}"/>
+    <hyperlink ref="Y354" r:id="rId1042" xr:uid="{03758A41-7740-46FF-AF5F-3B6F3C553C6E}"/>
+    <hyperlink ref="W355" r:id="rId1043" xr:uid="{0D25D25B-D57E-4ABF-921B-F133AF732DCE}"/>
+    <hyperlink ref="Y355" r:id="rId1044" xr:uid="{F8173409-2684-4C6F-84DA-CB4C762A8C3B}"/>
+    <hyperlink ref="X354" r:id="rId1045" xr:uid="{606D9ED5-EA36-4DC7-B6AE-6DA922DAD175}"/>
+    <hyperlink ref="X355" r:id="rId1046" xr:uid="{854387C7-0B2C-405E-AAE3-B67F1F7D067C}"/>
+    <hyperlink ref="W356" r:id="rId1047" xr:uid="{1627DE2F-0F8F-4C6E-8A9F-1BEABAFA5804}"/>
+    <hyperlink ref="Y356" r:id="rId1048" xr:uid="{1B976771-CDCE-4E08-8716-0F987504D0A3}"/>
+    <hyperlink ref="W357" r:id="rId1049" xr:uid="{3A823B3C-D0B0-4205-A5B8-085A73D5EDB6}"/>
+    <hyperlink ref="Y357" r:id="rId1050" xr:uid="{62EA34F2-82CD-45F8-811D-116516299058}"/>
+    <hyperlink ref="Y358" r:id="rId1051" xr:uid="{AD9958D9-41BA-4496-A208-88E7AE048673}"/>
+    <hyperlink ref="Y359" r:id="rId1052" xr:uid="{30690D40-D6EE-41A6-9CC4-99894435449D}"/>
+    <hyperlink ref="Y360" r:id="rId1053" xr:uid="{76914A48-0960-4C65-B365-F87E7B7A9B82}"/>
+    <hyperlink ref="Y361" r:id="rId1054" xr:uid="{9E2B3F81-BDE4-4CF3-ACF8-23B171DBFE0C}"/>
+    <hyperlink ref="X356" r:id="rId1055" xr:uid="{F513E14B-E317-45D0-9BF9-A2AF0B153E2E}"/>
+    <hyperlink ref="X357" r:id="rId1056" xr:uid="{907A5380-4193-411A-9A7F-88B1576B16CA}"/>
+    <hyperlink ref="X359" r:id="rId1057" xr:uid="{2F2E1A12-B49D-4E15-AB0B-B0F9AA8BAD99}"/>
+    <hyperlink ref="W359" r:id="rId1058" xr:uid="{5C01579D-DCF0-4FBA-9536-7CEBC2D9E3FC}"/>
+    <hyperlink ref="X360" r:id="rId1059" xr:uid="{9FAB48CF-2817-46CA-8484-DFA162CCEE2F}"/>
+    <hyperlink ref="W361" r:id="rId1060" xr:uid="{3757D6E3-985E-4709-89B5-874BF03F6ED5}"/>
+    <hyperlink ref="X361" r:id="rId1061" xr:uid="{FA88C2AA-8832-4EDA-B9E7-FC538C76D014}"/>
+    <hyperlink ref="W362" r:id="rId1062" xr:uid="{DA4AD43F-7E25-482A-9393-49D9D81DAC2E}"/>
+    <hyperlink ref="Y362" r:id="rId1063" xr:uid="{0E2D5724-F19E-41DE-8B65-1330AA48B241}"/>
+    <hyperlink ref="W363" r:id="rId1064" xr:uid="{44D291C2-2458-46E1-9891-24D93353538D}"/>
+    <hyperlink ref="Y363" r:id="rId1065" xr:uid="{2FA99855-933C-4C7A-9FF4-2B5BC22ABAB3}"/>
+    <hyperlink ref="W364" r:id="rId1066" xr:uid="{FDAFB492-222C-4146-8EFF-231147A6912C}"/>
+    <hyperlink ref="Y364" r:id="rId1067" xr:uid="{5D6ED7AA-0B58-4AAE-A9E7-A87E967EF63F}"/>
+    <hyperlink ref="W365" r:id="rId1068" xr:uid="{3681B67B-E4BF-4B1B-94B5-C0104BDE7103}"/>
+    <hyperlink ref="Y365" r:id="rId1069" xr:uid="{B103C372-CE54-49A2-A2C2-54E6F0D9D95C}"/>
+    <hyperlink ref="W366" r:id="rId1070" xr:uid="{225D158A-98FE-42F1-956E-95DB0B965D59}"/>
+    <hyperlink ref="Y366" r:id="rId1071" xr:uid="{CFA27551-6555-4F06-B1AD-DE81CFABB94B}"/>
+    <hyperlink ref="X362" r:id="rId1072" xr:uid="{85B4267D-1A98-45C7-9431-613EC78D9652}"/>
+    <hyperlink ref="X363" r:id="rId1073" xr:uid="{E8FA8DB4-2549-4FF0-B554-DA279CA038A7}"/>
+    <hyperlink ref="X364" r:id="rId1074" xr:uid="{611D9497-0ABC-4558-9C59-A46FBBF3378D}"/>
+    <hyperlink ref="X365" r:id="rId1075" xr:uid="{9229FC91-8A6E-4925-86F9-98E1EC8374F4}"/>
+    <hyperlink ref="X366" r:id="rId1076" xr:uid="{70F8D9D1-5D44-40B5-9AAA-79403C57AD02}"/>
+    <hyperlink ref="W367" r:id="rId1077" xr:uid="{DF5196D3-C0F8-4743-AA1A-806DB7144A30}"/>
+    <hyperlink ref="Y367" r:id="rId1078" xr:uid="{F7D2C4C4-EE3C-40EE-924B-C283DCA7661E}"/>
+    <hyperlink ref="W368" r:id="rId1079" xr:uid="{8386FAD3-4ADD-4DEF-A3F1-4082227DCD7D}"/>
+    <hyperlink ref="Y368" r:id="rId1080" xr:uid="{1CBAB3B8-1352-4CDD-8039-787BC54139B4}"/>
+    <hyperlink ref="Y369" r:id="rId1081" xr:uid="{B5B04103-83AF-481D-AE30-7F7412BBF61D}"/>
+    <hyperlink ref="W370" r:id="rId1082" xr:uid="{4E7053E9-66B0-4D6C-9E1D-8267CC893955}"/>
+    <hyperlink ref="Y370" r:id="rId1083" xr:uid="{F85962DE-0A0E-4841-99B9-DF5AB5E9D2ED}"/>
+    <hyperlink ref="W371" r:id="rId1084" xr:uid="{2B205E70-37F2-4E18-93C7-F4FAAA96BD4F}"/>
+    <hyperlink ref="Y371" r:id="rId1085" xr:uid="{E9AF1EA5-BBA6-428A-B625-138633326B72}"/>
+    <hyperlink ref="W372" r:id="rId1086" xr:uid="{A01B08C7-5BFA-4E57-A587-AC09D14C0861}"/>
+    <hyperlink ref="Y372" r:id="rId1087" xr:uid="{E14CAA8D-5674-4AFF-9C2A-28D106759D8E}"/>
+    <hyperlink ref="X367" r:id="rId1088" xr:uid="{7AD08E42-3348-4C99-B49C-F8205ED15D2D}"/>
+    <hyperlink ref="X368" r:id="rId1089" xr:uid="{4714B2C5-87BE-4EDA-8DDD-9239678A9C7B}"/>
+    <hyperlink ref="W369" r:id="rId1090" xr:uid="{CFC5BE56-15C8-4FE7-8071-C1020A728372}"/>
+    <hyperlink ref="X369" r:id="rId1091" xr:uid="{1FEF9C02-E7AA-41FE-B488-B46502DBA57B}"/>
+    <hyperlink ref="X371" r:id="rId1092" xr:uid="{34060A72-5CA7-4518-A0FD-B1529C91AD14}"/>
+    <hyperlink ref="X372" r:id="rId1093" xr:uid="{DF0E72E0-568F-4BB3-B2CB-8C9155094A92}"/>
+    <hyperlink ref="W373" r:id="rId1094" xr:uid="{570D4878-C4D0-400D-84A8-18D1470424E1}"/>
+    <hyperlink ref="Y373" r:id="rId1095" xr:uid="{602FB456-A2F5-4B10-8959-7A9BAB1ED601}"/>
+    <hyperlink ref="X373" r:id="rId1096" xr:uid="{31FD147F-B3E2-4793-A7C3-2B6465302BE9}"/>
+    <hyperlink ref="W374" r:id="rId1097" xr:uid="{17E32179-074D-4168-A516-BBC55DDC9484}"/>
+    <hyperlink ref="Y374" r:id="rId1098" xr:uid="{1AD27D10-FA47-427D-9C5B-2A50F399F04E}"/>
+    <hyperlink ref="X374" r:id="rId1099" xr:uid="{611FEF65-5E67-456C-BF6D-28756EE03364}"/>
+    <hyperlink ref="W375" r:id="rId1100" xr:uid="{E427FB9E-62A4-4D4C-91D7-3EA2B7AA2873}"/>
+    <hyperlink ref="Y375" r:id="rId1101" xr:uid="{1FEEC613-8DEA-4361-8656-5AE8FB912639}"/>
+    <hyperlink ref="W376" r:id="rId1102" xr:uid="{F915E7CC-0928-440D-9415-0003916A2700}"/>
+    <hyperlink ref="Y376" r:id="rId1103" xr:uid="{36745C78-BFC2-4285-A987-392EA80D7F06}"/>
+    <hyperlink ref="X375" r:id="rId1104" xr:uid="{2DF89CDE-07E1-4613-B849-900424B0BE98}"/>
+    <hyperlink ref="X376" r:id="rId1105" xr:uid="{B038BC66-F595-4BD3-924A-55E50B2C3EA3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>